<commit_message>
Updating files for August 31
</commit_message>
<xml_diff>
--- a/assets/Historical_Starting_Pitchers.xlsx
+++ b/assets/Historical_Starting_Pitchers.xlsx
@@ -25,6 +25,93 @@
     <t>Handedness</t>
   </si>
   <si>
+    <t>Andre Pallante</t>
+  </si>
+  <si>
+    <t>Brady Singer</t>
+  </si>
+  <si>
+    <t>Brandon Pfaadt</t>
+  </si>
+  <si>
+    <t>Brandon Woodruff</t>
+  </si>
+  <si>
+    <t>Bryce Miller</t>
+  </si>
+  <si>
+    <t>Hunter Brown</t>
+  </si>
+  <si>
+    <t>Hurston Waldrep</t>
+  </si>
+  <si>
+    <t>J T Ginn</t>
+  </si>
+  <si>
+    <t>Jacob deGrom</t>
+  </si>
+  <si>
+    <t>Jesus Luzardo</t>
+  </si>
+  <si>
+    <t>Joe Ryan</t>
+  </si>
+  <si>
+    <t>José Soriano</t>
+  </si>
+  <si>
+    <t>Justin Verlander</t>
+  </si>
+  <si>
+    <t>Kodai Senga</t>
+  </si>
+  <si>
+    <t>Lucas Giolito</t>
+  </si>
+  <si>
+    <t>Luis Gil</t>
+  </si>
+  <si>
+    <t>Martín Pérez</t>
+  </si>
+  <si>
+    <t>Matthew Boyd</t>
+  </si>
+  <si>
+    <t>Max Scherzer</t>
+  </si>
+  <si>
+    <t>Michael Wacha</t>
+  </si>
+  <si>
+    <t>Mitch Keller</t>
+  </si>
+  <si>
+    <t>Sandy Alcantara</t>
+  </si>
+  <si>
+    <t>Tanner Bibee</t>
+  </si>
+  <si>
+    <t>Tanner Gordon</t>
+  </si>
+  <si>
+    <t>Tarik Skubal</t>
+  </si>
+  <si>
+    <t>Yoshinobu Yamamoto</t>
+  </si>
+  <si>
+    <t>Tomoyuki Sugano</t>
+  </si>
+  <si>
+    <t>Brad Lord</t>
+  </si>
+  <si>
+    <t>Ian Seymour</t>
+  </si>
+  <si>
     <t>Andrew Abbott</t>
   </si>
   <si>
@@ -340,15 +427,9 @@
     <t>Luis Morales</t>
   </si>
   <si>
-    <t>Andre Pallante</t>
-  </si>
-  <si>
     <t>Bailey Ober</t>
   </si>
   <si>
-    <t>Brandon Pfaadt</t>
-  </si>
-  <si>
     <t>Charlie Morton</t>
   </si>
   <si>
@@ -361,45 +442,18 @@
     <t>Dylan Cease</t>
   </si>
   <si>
-    <t>Hunter Brown</t>
-  </si>
-  <si>
-    <t>Hurston Waldrep</t>
-  </si>
-  <si>
-    <t>Jesus Luzardo</t>
-  </si>
-  <si>
-    <t>Justin Verlander</t>
-  </si>
-  <si>
     <t>Kyle Bradish</t>
   </si>
   <si>
-    <t>Lucas Giolito</t>
-  </si>
-  <si>
     <t>Luis Castillo</t>
   </si>
   <si>
-    <t>Luis Gil</t>
-  </si>
-  <si>
     <t>MacKenzie Gore</t>
   </si>
   <si>
-    <t>Martín Pérez</t>
-  </si>
-  <si>
-    <t>Matthew Boyd</t>
-  </si>
-  <si>
     <t>Michael Lorenzen</t>
   </si>
   <si>
-    <t>Mitch Keller</t>
-  </si>
-  <si>
     <t>Nick Martinez</t>
   </si>
   <si>
@@ -409,18 +463,12 @@
     <t>Patrick Corbin</t>
   </si>
   <si>
-    <t>Sandy Alcantara</t>
-  </si>
-  <si>
     <t>Sean Manaea</t>
   </si>
   <si>
     <t>Shane Baz</t>
   </si>
   <si>
-    <t>Tanner Gordon</t>
-  </si>
-  <si>
     <t>Yusei Kikuchi</t>
   </si>
   <si>
@@ -430,75 +478,30 @@
     <t>Parker Messick</t>
   </si>
   <si>
-    <t>Brandon Woodruff</t>
-  </si>
-  <si>
-    <t>Bryce Miller</t>
-  </si>
-  <si>
     <t>Emmet Sheehan</t>
   </si>
   <si>
     <t>Hunter Greene</t>
   </si>
   <si>
-    <t>J T Ginn</t>
-  </si>
-  <si>
-    <t>Jacob deGrom</t>
-  </si>
-  <si>
-    <t>Joe Ryan</t>
-  </si>
-  <si>
-    <t>José Soriano</t>
-  </si>
-  <si>
     <t>JP Sears</t>
   </si>
   <si>
-    <t>Kodai Senga</t>
-  </si>
-  <si>
-    <t>Max Scherzer</t>
-  </si>
-  <si>
     <t>Richard Fitts</t>
   </si>
   <si>
     <t>Spencer Strider</t>
   </si>
   <si>
-    <t>Tanner Bibee</t>
-  </si>
-  <si>
-    <t>Tarik Skubal</t>
-  </si>
-  <si>
-    <t>Tomoyuki Sugano</t>
-  </si>
-  <si>
-    <t>Brad Lord</t>
-  </si>
-  <si>
     <t>Noah Cameron</t>
   </si>
   <si>
-    <t>Ian Seymour</t>
-  </si>
-  <si>
-    <t>Brady Singer</t>
-  </si>
-  <si>
     <t>Jameson Taillon</t>
   </si>
   <si>
     <t>Robert Gasser</t>
   </si>
   <si>
-    <t>Yoshinobu Yamamoto</t>
-  </si>
-  <si>
     <t>Jacob Lopez</t>
   </si>
   <si>
@@ -508,9 +511,6 @@
     <t>José Berríos</t>
   </si>
   <si>
-    <t>Michael Wacha</t>
-  </si>
-  <si>
     <t>Mick Abel</t>
   </si>
   <si>
@@ -832,10 +832,10 @@
     <t>Nathan Wiles</t>
   </si>
   <si>
+    <t>RHP</t>
+  </si>
+  <si>
     <t>LHP</t>
-  </si>
-  <si>
-    <t>RHP</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1215,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>671096</v>
+        <v>669467</v>
       </c>
       <c r="C2" t="s">
         <v>272</v>
@@ -1226,7 +1226,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>519242</v>
+        <v>663903</v>
       </c>
       <c r="C3" t="s">
         <v>272</v>
@@ -1237,7 +1237,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>650911</v>
+        <v>694297</v>
       </c>
       <c r="C4" t="s">
         <v>272</v>
@@ -1248,7 +1248,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>656849</v>
+        <v>605540</v>
       </c>
       <c r="C5" t="s">
         <v>272</v>
@@ -1259,10 +1259,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>669160</v>
+        <v>682243</v>
       </c>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1270,7 +1270,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>593958</v>
+        <v>686613</v>
       </c>
       <c r="C7" t="s">
         <v>272</v>
@@ -1281,10 +1281,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>665795</v>
+        <v>694462</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1292,10 +1292,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>668909</v>
+        <v>669372</v>
       </c>
       <c r="C9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1303,10 +1303,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>656427</v>
+        <v>594798</v>
       </c>
       <c r="C10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1314,7 +1314,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>663623</v>
+        <v>666200</v>
       </c>
       <c r="C11" t="s">
         <v>273</v>
@@ -1325,10 +1325,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>665871</v>
+        <v>657746</v>
       </c>
       <c r="C12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1336,10 +1336,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>670912</v>
+        <v>667755</v>
       </c>
       <c r="C13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1347,10 +1347,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>592332</v>
+        <v>434378</v>
       </c>
       <c r="C14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1358,51 +1358,45 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>543294</v>
+        <v>673540</v>
       </c>
       <c r="C15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>669302</v>
-      </c>
       <c r="C16" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>518876</v>
+        <v>608337</v>
       </c>
       <c r="C17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>700241</v>
+        <v>661563</v>
       </c>
       <c r="C18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>601713</v>
+        <v>527048</v>
       </c>
       <c r="C19" t="s">
         <v>273</v>
@@ -1410,10 +1404,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>682990</v>
+        <v>571510</v>
       </c>
       <c r="C20" t="s">
         <v>273</v>
@@ -1421,43 +1415,43 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>686752</v>
+        <v>453286</v>
       </c>
       <c r="C21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
-        <v>681293</v>
+        <v>608379</v>
       </c>
       <c r="C22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>671737</v>
+        <v>656605</v>
       </c>
       <c r="C23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>669432</v>
+        <v>645261</v>
       </c>
       <c r="C24" t="s">
         <v>272</v>
@@ -1465,32 +1459,32 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>607192</v>
+        <v>676440</v>
       </c>
       <c r="C25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>681343</v>
+        <v>685299</v>
       </c>
       <c r="C26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>663568</v>
+        <v>669373</v>
       </c>
       <c r="C27" t="s">
         <v>273</v>
@@ -1498,43 +1492,43 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>693645</v>
+        <v>808967</v>
       </c>
       <c r="C28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>693313</v>
+        <v>608372</v>
       </c>
       <c r="C29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30">
-        <v>685326</v>
+        <v>695418</v>
       </c>
       <c r="C30" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>686930</v>
+        <v>693855</v>
       </c>
       <c r="C31" t="s">
         <v>273</v>
@@ -1542,10 +1536,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32">
-        <v>605288</v>
+        <v>671096</v>
       </c>
       <c r="C32" t="s">
         <v>273</v>
@@ -1553,21 +1547,21 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33">
-        <v>605483</v>
+        <v>519242</v>
       </c>
       <c r="C33" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34">
-        <v>693821</v>
+        <v>650911</v>
       </c>
       <c r="C34" t="s">
         <v>273</v>
@@ -1575,32 +1569,32 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
-        <v>607074</v>
+        <v>656849</v>
       </c>
       <c r="C35" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36">
-        <v>663978</v>
+        <v>669160</v>
       </c>
       <c r="C36" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37">
-        <v>664299</v>
+        <v>593958</v>
       </c>
       <c r="C37" t="s">
         <v>273</v>
@@ -1608,76 +1602,76 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38">
-        <v>665152</v>
+        <v>665795</v>
       </c>
       <c r="C38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39">
-        <v>691587</v>
+        <v>668909</v>
       </c>
       <c r="C39" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40">
-        <v>642547</v>
+        <v>656427</v>
       </c>
       <c r="C40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41">
-        <v>669923</v>
+        <v>663623</v>
       </c>
       <c r="C41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42">
-        <v>608566</v>
+        <v>665871</v>
       </c>
       <c r="C42" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43">
-        <v>683004</v>
+        <v>670912</v>
       </c>
       <c r="C43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44">
-        <v>605488</v>
+        <v>592332</v>
       </c>
       <c r="C44" t="s">
         <v>272</v>
@@ -1685,10 +1679,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45">
-        <v>671106</v>
+        <v>543294</v>
       </c>
       <c r="C45" t="s">
         <v>272</v>
@@ -1696,10 +1690,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46">
-        <v>669461</v>
+        <v>669302</v>
       </c>
       <c r="C46" t="s">
         <v>272</v>
@@ -1707,10 +1701,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47">
-        <v>680730</v>
+        <v>518876</v>
       </c>
       <c r="C47" t="s">
         <v>272</v>
@@ -1718,10 +1712,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48">
-        <v>641482</v>
+        <v>700241</v>
       </c>
       <c r="C48" t="s">
         <v>272</v>
@@ -1729,21 +1723,21 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49">
-        <v>694973</v>
+        <v>601713</v>
       </c>
       <c r="C49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50">
-        <v>624133</v>
+        <v>682990</v>
       </c>
       <c r="C50" t="s">
         <v>272</v>
@@ -1751,10 +1745,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51">
-        <v>592662</v>
+        <v>686752</v>
       </c>
       <c r="C51" t="s">
         <v>272</v>
@@ -1762,98 +1756,98 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52">
-        <v>607625</v>
+        <v>681293</v>
       </c>
       <c r="C52" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53">
-        <v>669456</v>
+        <v>671737</v>
       </c>
       <c r="C53" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54">
-        <v>542881</v>
+        <v>669432</v>
       </c>
       <c r="C54" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55">
-        <v>668678</v>
+        <v>607192</v>
       </c>
       <c r="C55" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56">
-        <v>641793</v>
+        <v>681343</v>
       </c>
       <c r="C56" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57">
-        <v>805673</v>
+        <v>663568</v>
       </c>
       <c r="C57" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58">
-        <v>690990</v>
+        <v>693645</v>
       </c>
       <c r="C58" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59">
-        <v>672782</v>
+        <v>693313</v>
       </c>
       <c r="C59" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60">
-        <v>801139</v>
+        <v>685326</v>
       </c>
       <c r="C60" t="s">
         <v>272</v>
@@ -1861,32 +1855,32 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61">
-        <v>804636</v>
+        <v>686930</v>
       </c>
       <c r="C61" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62">
-        <v>605400</v>
+        <v>605288</v>
       </c>
       <c r="C62" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63">
-        <v>800049</v>
+        <v>605483</v>
       </c>
       <c r="C63" t="s">
         <v>273</v>
@@ -1894,10 +1888,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64">
-        <v>700249</v>
+        <v>693821</v>
       </c>
       <c r="C64" t="s">
         <v>272</v>
@@ -1905,10 +1899,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65">
-        <v>615698</v>
+        <v>607074</v>
       </c>
       <c r="C65" t="s">
         <v>273</v>
@@ -1916,32 +1910,32 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66">
-        <v>605280</v>
+        <v>663978</v>
       </c>
       <c r="C66" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67">
-        <v>663436</v>
+        <v>664299</v>
       </c>
       <c r="C67" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68">
-        <v>676979</v>
+        <v>665152</v>
       </c>
       <c r="C68" t="s">
         <v>272</v>
@@ -1949,10 +1943,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69">
-        <v>500779</v>
+        <v>691587</v>
       </c>
       <c r="C69" t="s">
         <v>272</v>
@@ -1960,10 +1954,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70">
-        <v>607536</v>
+        <v>642547</v>
       </c>
       <c r="C70" t="s">
         <v>272</v>
@@ -1971,54 +1965,54 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71">
-        <v>657277</v>
+        <v>669923</v>
       </c>
       <c r="C71" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72">
-        <v>571945</v>
+        <v>608566</v>
       </c>
       <c r="C72" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73">
-        <v>622503</v>
+        <v>683004</v>
       </c>
       <c r="C73" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74">
-        <v>684007</v>
+        <v>605488</v>
       </c>
       <c r="C74" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75">
-        <v>701542</v>
+        <v>671106</v>
       </c>
       <c r="C75" t="s">
         <v>273</v>
@@ -2026,10 +2020,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76">
-        <v>669920</v>
+        <v>669461</v>
       </c>
       <c r="C76" t="s">
         <v>273</v>
@@ -2037,10 +2031,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77">
-        <v>677952</v>
+        <v>680730</v>
       </c>
       <c r="C77" t="s">
         <v>273</v>
@@ -2048,10 +2042,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78">
-        <v>650644</v>
+        <v>641482</v>
       </c>
       <c r="C78" t="s">
         <v>273</v>
@@ -2059,21 +2053,21 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B79">
-        <v>678394</v>
+        <v>694973</v>
       </c>
       <c r="C79" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B80">
-        <v>693433</v>
+        <v>624133</v>
       </c>
       <c r="C80" t="s">
         <v>273</v>
@@ -2081,10 +2075,10 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81">
-        <v>676917</v>
+        <v>592662</v>
       </c>
       <c r="C81" t="s">
         <v>273</v>
@@ -2092,10 +2086,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82">
-        <v>687931</v>
+        <v>607625</v>
       </c>
       <c r="C82" t="s">
         <v>272</v>
@@ -2103,21 +2097,21 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B83">
-        <v>663554</v>
+        <v>669456</v>
       </c>
       <c r="C83" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B84">
-        <v>607067</v>
+        <v>542881</v>
       </c>
       <c r="C84" t="s">
         <v>273</v>
@@ -2125,21 +2119,21 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85">
-        <v>656876</v>
+        <v>668678</v>
       </c>
       <c r="C85" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B86">
-        <v>641778</v>
+        <v>641793</v>
       </c>
       <c r="C86" t="s">
         <v>272</v>
@@ -2147,10 +2141,10 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87">
-        <v>664285</v>
+        <v>805673</v>
       </c>
       <c r="C87" t="s">
         <v>272</v>
@@ -2158,21 +2152,21 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B88">
-        <v>686799</v>
+        <v>690990</v>
       </c>
       <c r="C88" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89">
-        <v>666214</v>
+        <v>672782</v>
       </c>
       <c r="C89" t="s">
         <v>272</v>
@@ -2180,21 +2174,21 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B90">
-        <v>608331</v>
+        <v>801139</v>
       </c>
       <c r="C90" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91">
-        <v>666157</v>
+        <v>804636</v>
       </c>
       <c r="C91" t="s">
         <v>272</v>
@@ -2202,32 +2196,32 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B92">
-        <v>672710</v>
+        <v>605400</v>
       </c>
       <c r="C92" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93">
-        <v>669194</v>
+        <v>800049</v>
       </c>
       <c r="C93" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94">
-        <v>660271</v>
+        <v>700249</v>
       </c>
       <c r="C94" t="s">
         <v>273</v>
@@ -2235,43 +2229,43 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B95">
-        <v>680573</v>
+        <v>615698</v>
       </c>
       <c r="C95" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B96">
-        <v>677944</v>
+        <v>605280</v>
       </c>
       <c r="C96" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B97">
-        <v>543243</v>
+        <v>663436</v>
       </c>
       <c r="C97" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B98">
-        <v>592836</v>
+        <v>676979</v>
       </c>
       <c r="C98" t="s">
         <v>273</v>
@@ -2279,10 +2273,10 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B99">
-        <v>506433</v>
+        <v>500779</v>
       </c>
       <c r="C99" t="s">
         <v>273</v>
@@ -2290,10 +2284,10 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B100">
-        <v>801403</v>
+        <v>607536</v>
       </c>
       <c r="C100" t="s">
         <v>273</v>
@@ -2301,32 +2295,32 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B101">
-        <v>687473</v>
+        <v>657277</v>
       </c>
       <c r="C101" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B102">
-        <v>686701</v>
+        <v>571945</v>
       </c>
       <c r="C102" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B103">
-        <v>656641</v>
+        <v>622503</v>
       </c>
       <c r="C103" t="s">
         <v>272</v>
@@ -2334,10 +2328,10 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B104">
-        <v>690997</v>
+        <v>684007</v>
       </c>
       <c r="C104" t="s">
         <v>273</v>
@@ -2345,142 +2339,142 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B105">
-        <v>696149</v>
+        <v>701542</v>
       </c>
       <c r="C105" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B106">
-        <v>806960</v>
+        <v>669920</v>
       </c>
       <c r="C106" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B107">
-        <v>669467</v>
+        <v>677952</v>
       </c>
       <c r="C107" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B108">
-        <v>641927</v>
+        <v>650644</v>
       </c>
       <c r="C108" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B109">
-        <v>694297</v>
+        <v>678394</v>
       </c>
       <c r="C109" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B110">
-        <v>450203</v>
+        <v>693433</v>
       </c>
       <c r="C110" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B111">
-        <v>605135</v>
+        <v>676917</v>
       </c>
       <c r="C111" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B112">
-        <v>477132</v>
+        <v>687931</v>
       </c>
       <c r="C112" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B113">
-        <v>656302</v>
+        <v>663554</v>
       </c>
       <c r="C113" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B114">
-        <v>686613</v>
+        <v>607067</v>
       </c>
       <c r="C114" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B115">
-        <v>694462</v>
+        <v>656876</v>
       </c>
       <c r="C115" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B116">
-        <v>666200</v>
+        <v>641778</v>
       </c>
       <c r="C116" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B117">
-        <v>434378</v>
+        <v>664285</v>
       </c>
       <c r="C117" t="s">
         <v>273</v>
@@ -2488,21 +2482,21 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B118">
-        <v>680694</v>
+        <v>686799</v>
       </c>
       <c r="C118" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B119">
-        <v>608337</v>
+        <v>666214</v>
       </c>
       <c r="C119" t="s">
         <v>273</v>
@@ -2510,10 +2504,10 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B120">
-        <v>622491</v>
+        <v>608331</v>
       </c>
       <c r="C120" t="s">
         <v>273</v>
@@ -2521,10 +2515,10 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B121">
-        <v>661563</v>
+        <v>666157</v>
       </c>
       <c r="C121" t="s">
         <v>273</v>
@@ -2532,10 +2526,10 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B122">
-        <v>669022</v>
+        <v>672710</v>
       </c>
       <c r="C122" t="s">
         <v>272</v>
@@ -2543,10 +2537,10 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B123">
-        <v>527048</v>
+        <v>669194</v>
       </c>
       <c r="C123" t="s">
         <v>272</v>
@@ -2554,10 +2548,10 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B124">
-        <v>571510</v>
+        <v>660271</v>
       </c>
       <c r="C124" t="s">
         <v>272</v>
@@ -2565,54 +2559,54 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B125">
-        <v>547179</v>
+        <v>680573</v>
       </c>
       <c r="C125" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B126">
-        <v>656605</v>
+        <v>677944</v>
       </c>
       <c r="C126" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B127">
-        <v>607259</v>
+        <v>543243</v>
       </c>
       <c r="C127" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B128">
-        <v>674370</v>
+        <v>592836</v>
       </c>
       <c r="C128" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B129">
-        <v>571578</v>
+        <v>506433</v>
       </c>
       <c r="C129" t="s">
         <v>272</v>
@@ -2620,21 +2614,21 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B130">
-        <v>645261</v>
+        <v>801403</v>
       </c>
       <c r="C130" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B131">
-        <v>640455</v>
+        <v>687473</v>
       </c>
       <c r="C131" t="s">
         <v>272</v>
@@ -2642,21 +2636,21 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B132">
-        <v>669358</v>
+        <v>686701</v>
       </c>
       <c r="C132" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B133">
-        <v>685299</v>
+        <v>656641</v>
       </c>
       <c r="C133" t="s">
         <v>273</v>
@@ -2664,10 +2658,10 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B134">
-        <v>579328</v>
+        <v>690997</v>
       </c>
       <c r="C134" t="s">
         <v>272</v>
@@ -2675,21 +2669,21 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B135">
-        <v>694819</v>
+        <v>696149</v>
       </c>
       <c r="C135" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B136">
-        <v>800048</v>
+        <v>806960</v>
       </c>
       <c r="C136" t="s">
         <v>272</v>
@@ -2697,43 +2691,43 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B137">
-        <v>605540</v>
+        <v>641927</v>
       </c>
       <c r="C137" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B138">
-        <v>682243</v>
+        <v>450203</v>
       </c>
       <c r="C138" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B139">
-        <v>686218</v>
+        <v>605135</v>
       </c>
       <c r="C139" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B140">
-        <v>668881</v>
+        <v>477132</v>
       </c>
       <c r="C140" t="s">
         <v>273</v>
@@ -2741,43 +2735,43 @@
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B141">
-        <v>669372</v>
+        <v>656302</v>
       </c>
       <c r="C141" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B142">
-        <v>594798</v>
+        <v>680694</v>
       </c>
       <c r="C142" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B143">
-        <v>657746</v>
+        <v>622491</v>
       </c>
       <c r="C143" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B144">
-        <v>667755</v>
+        <v>669022</v>
       </c>
       <c r="C144" t="s">
         <v>273</v>
@@ -2785,10 +2779,10 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B145">
-        <v>676664</v>
+        <v>547179</v>
       </c>
       <c r="C145" t="s">
         <v>272</v>
@@ -2796,32 +2790,32 @@
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B146">
-        <v>673540</v>
+        <v>607259</v>
       </c>
       <c r="C146" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B147">
-        <v>453286</v>
+        <v>674370</v>
       </c>
       <c r="C147" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B148">
-        <v>690916</v>
+        <v>571578</v>
       </c>
       <c r="C148" t="s">
         <v>273</v>
@@ -2829,10 +2823,10 @@
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B149">
-        <v>675911</v>
+        <v>640455</v>
       </c>
       <c r="C149" t="s">
         <v>273</v>
@@ -2840,43 +2834,43 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B150">
-        <v>676440</v>
+        <v>669358</v>
       </c>
       <c r="C150" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B151">
-        <v>669373</v>
+        <v>579328</v>
       </c>
       <c r="C151" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B152">
-        <v>608372</v>
+        <v>694819</v>
       </c>
       <c r="C152" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B153">
-        <v>695418</v>
+        <v>800048</v>
       </c>
       <c r="C153" t="s">
         <v>273</v>
@@ -2884,10 +2878,10 @@
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B154">
-        <v>702070</v>
+        <v>686218</v>
       </c>
       <c r="C154" t="s">
         <v>272</v>
@@ -2895,10 +2889,10 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B155">
-        <v>693855</v>
+        <v>668881</v>
       </c>
       <c r="C155" t="s">
         <v>272</v>
@@ -2906,18 +2900,24 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
+        <v>156</v>
+      </c>
+      <c r="B156">
+        <v>676664</v>
+      </c>
+      <c r="C156" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
         <v>157</v>
       </c>
-      <c r="B156">
-        <v>663903</v>
-      </c>
-      <c r="C156" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
+      <c r="B157">
+        <v>690916</v>
+      </c>
       <c r="C157" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2925,10 +2925,10 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>592791</v>
+        <v>675911</v>
       </c>
       <c r="C158" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2936,10 +2936,10 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>688107</v>
+        <v>702070</v>
       </c>
       <c r="C159" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2947,10 +2947,10 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>808967</v>
+        <v>592791</v>
       </c>
       <c r="C160" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2958,10 +2958,10 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>682052</v>
+        <v>688107</v>
       </c>
       <c r="C161" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2969,7 +2969,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>676083</v>
+        <v>682052</v>
       </c>
       <c r="C162" t="s">
         <v>273</v>
@@ -2980,10 +2980,10 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>621244</v>
+        <v>676083</v>
       </c>
       <c r="C163" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2991,10 +2991,10 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>608379</v>
+        <v>621244</v>
       </c>
       <c r="C164" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3005,7 +3005,7 @@
         <v>690953</v>
       </c>
       <c r="C165" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3016,7 +3016,7 @@
         <v>681347</v>
       </c>
       <c r="C166" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3027,7 +3027,7 @@
         <v>682929</v>
       </c>
       <c r="C167" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3038,7 +3038,7 @@
         <v>671212</v>
       </c>
       <c r="C168" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3049,7 +3049,7 @@
         <v>570632</v>
       </c>
       <c r="C169" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3060,7 +3060,7 @@
         <v>687064</v>
       </c>
       <c r="C170" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3071,7 +3071,7 @@
         <v>678022</v>
       </c>
       <c r="C171" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3082,7 +3082,7 @@
         <v>689017</v>
       </c>
       <c r="C172" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3093,15 +3093,15 @@
         <v>596295</v>
       </c>
       <c r="C173" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="C174" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3112,7 +3112,7 @@
         <v>621111</v>
       </c>
       <c r="C175" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3123,7 +3123,7 @@
         <v>694477</v>
       </c>
       <c r="C176" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3134,7 +3134,7 @@
         <v>678906</v>
       </c>
       <c r="C177" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3145,7 +3145,7 @@
         <v>571760</v>
       </c>
       <c r="C178" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3156,7 +3156,7 @@
         <v>607200</v>
       </c>
       <c r="C179" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3167,7 +3167,7 @@
         <v>543135</v>
       </c>
       <c r="C180" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3178,7 +3178,7 @@
         <v>471911</v>
       </c>
       <c r="C181" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3189,7 +3189,7 @@
         <v>663559</v>
       </c>
       <c r="C182" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3200,7 +3200,7 @@
         <v>647336</v>
       </c>
       <c r="C183" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3211,7 +3211,7 @@
         <v>701519</v>
       </c>
       <c r="C184" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3222,7 +3222,7 @@
         <v>677958</v>
       </c>
       <c r="C185" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3233,7 +3233,7 @@
         <v>573186</v>
       </c>
       <c r="C186" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3244,7 +3244,7 @@
         <v>686563</v>
       </c>
       <c r="C187" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3255,7 +3255,7 @@
         <v>622663</v>
       </c>
       <c r="C188" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3266,7 +3266,7 @@
         <v>687922</v>
       </c>
       <c r="C189" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3277,7 +3277,7 @@
         <v>688138</v>
       </c>
       <c r="C190" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3288,7 +3288,7 @@
         <v>701487</v>
       </c>
       <c r="C191" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3299,7 +3299,7 @@
         <v>687134</v>
       </c>
       <c r="C192" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3310,7 +3310,7 @@
         <v>593423</v>
       </c>
       <c r="C193" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3321,7 +3321,7 @@
         <v>448179</v>
       </c>
       <c r="C194" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3332,7 +3332,7 @@
         <v>621107</v>
       </c>
       <c r="C195" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3343,7 +3343,7 @@
         <v>695505</v>
       </c>
       <c r="C196" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3354,7 +3354,7 @@
         <v>675512</v>
       </c>
       <c r="C197" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3365,7 +3365,7 @@
         <v>676962</v>
       </c>
       <c r="C198" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3376,7 +3376,7 @@
         <v>676282</v>
       </c>
       <c r="C199" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3387,7 +3387,7 @@
         <v>680732</v>
       </c>
       <c r="C200" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3398,7 +3398,7 @@
         <v>554430</v>
       </c>
       <c r="C201" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3409,7 +3409,7 @@
         <v>676467</v>
       </c>
       <c r="C202" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3420,7 +3420,7 @@
         <v>656550</v>
       </c>
       <c r="C203" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3431,7 +3431,7 @@
         <v>663460</v>
       </c>
       <c r="C204" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3442,7 +3442,7 @@
         <v>681190</v>
       </c>
       <c r="C205" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3453,7 +3453,7 @@
         <v>669721</v>
       </c>
       <c r="C206" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3464,7 +3464,7 @@
         <v>701581</v>
       </c>
       <c r="C207" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3475,7 +3475,7 @@
         <v>806185</v>
       </c>
       <c r="C208" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3486,7 +3486,7 @@
         <v>672456</v>
       </c>
       <c r="C209" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3497,7 +3497,7 @@
         <v>687888</v>
       </c>
       <c r="C210" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -3508,7 +3508,7 @@
         <v>681857</v>
       </c>
       <c r="C211" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3519,7 +3519,7 @@
         <v>666171</v>
       </c>
       <c r="C212" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3530,7 +3530,7 @@
         <v>663795</v>
       </c>
       <c r="C213" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3541,7 +3541,7 @@
         <v>696136</v>
       </c>
       <c r="C214" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3552,7 +3552,7 @@
         <v>680736</v>
       </c>
       <c r="C215" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3563,7 +3563,7 @@
         <v>642216</v>
       </c>
       <c r="C216" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3574,7 +3574,7 @@
         <v>621112</v>
       </c>
       <c r="C217" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3585,7 +3585,7 @@
         <v>680885</v>
       </c>
       <c r="C218" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3596,7 +3596,7 @@
         <v>605513</v>
       </c>
       <c r="C219" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3607,7 +3607,7 @@
         <v>641302</v>
       </c>
       <c r="C220" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -3618,7 +3618,7 @@
         <v>690928</v>
       </c>
       <c r="C221" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3629,7 +3629,7 @@
         <v>694918</v>
       </c>
       <c r="C222" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3640,7 +3640,7 @@
         <v>800311</v>
       </c>
       <c r="C223" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3651,7 +3651,7 @@
         <v>592866</v>
       </c>
       <c r="C224" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3662,7 +3662,7 @@
         <v>678024</v>
       </c>
       <c r="C225" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3673,7 +3673,7 @@
         <v>642232</v>
       </c>
       <c r="C226" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3684,7 +3684,7 @@
         <v>669422</v>
       </c>
       <c r="C227" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3695,7 +3695,7 @@
         <v>657376</v>
       </c>
       <c r="C228" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3706,7 +3706,7 @@
         <v>676508</v>
       </c>
       <c r="C229" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3717,7 +3717,7 @@
         <v>687223</v>
       </c>
       <c r="C230" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3728,7 +3728,7 @@
         <v>656288</v>
       </c>
       <c r="C231" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3739,7 +3739,7 @@
         <v>690986</v>
       </c>
       <c r="C232" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3750,7 +3750,7 @@
         <v>687765</v>
       </c>
       <c r="C233" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3761,7 +3761,7 @@
         <v>641816</v>
       </c>
       <c r="C234" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3772,7 +3772,7 @@
         <v>687830</v>
       </c>
       <c r="C235" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3783,7 +3783,7 @@
         <v>676106</v>
       </c>
       <c r="C236" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3791,7 +3791,7 @@
         <v>236</v>
       </c>
       <c r="C237" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3802,7 +3802,7 @@
         <v>489119</v>
       </c>
       <c r="C238" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3813,7 +3813,7 @@
         <v>670102</v>
       </c>
       <c r="C239" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3821,7 +3821,7 @@
         <v>239</v>
       </c>
       <c r="C240" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3832,7 +3832,7 @@
         <v>656731</v>
       </c>
       <c r="C241" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3843,7 +3843,7 @@
         <v>676961</v>
       </c>
       <c r="C242" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3854,7 +3854,7 @@
         <v>677960</v>
       </c>
       <c r="C243" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3865,7 +3865,7 @@
         <v>605452</v>
       </c>
       <c r="C244" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3876,7 +3876,7 @@
         <v>666142</v>
       </c>
       <c r="C245" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3887,7 +3887,7 @@
         <v>689017</v>
       </c>
       <c r="C246" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3898,7 +3898,7 @@
         <v>664062</v>
       </c>
       <c r="C247" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3909,7 +3909,7 @@
         <v>676428</v>
       </c>
       <c r="C248" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3920,7 +3920,7 @@
         <v>641154</v>
       </c>
       <c r="C249" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3931,7 +3931,7 @@
         <v>676974</v>
       </c>
       <c r="C250" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3942,7 +3942,7 @@
         <v>669203</v>
       </c>
       <c r="C251" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3953,7 +3953,7 @@
         <v>680684</v>
       </c>
       <c r="C252" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3964,7 +3964,7 @@
         <v>700363</v>
       </c>
       <c r="C253" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -3975,7 +3975,7 @@
         <v>663465</v>
       </c>
       <c r="C254" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -3986,7 +3986,7 @@
         <v>695549</v>
       </c>
       <c r="C255" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -3997,7 +3997,7 @@
         <v>663738</v>
       </c>
       <c r="C256" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -4008,7 +4008,7 @@
         <v>701656</v>
       </c>
       <c r="C257" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -4019,7 +4019,7 @@
         <v>650633</v>
       </c>
       <c r="C258" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -4030,7 +4030,7 @@
         <v>694646</v>
       </c>
       <c r="C259" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -4041,7 +4041,7 @@
         <v>669060</v>
       </c>
       <c r="C260" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -4052,7 +4052,7 @@
         <v>669387</v>
       </c>
       <c r="C261" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -4063,7 +4063,7 @@
         <v>502043</v>
       </c>
       <c r="C262" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -4074,7 +4074,7 @@
         <v>669854</v>
       </c>
       <c r="C263" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -4085,7 +4085,7 @@
         <v>668964</v>
       </c>
       <c r="C264" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -4096,7 +4096,7 @@
         <v>695534</v>
       </c>
       <c r="C265" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -4107,7 +4107,7 @@
         <v>663855</v>
       </c>
       <c r="C266" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -4118,7 +4118,7 @@
         <v>678368</v>
       </c>
       <c r="C267" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -4129,7 +4129,7 @@
         <v>594902</v>
       </c>
       <c r="C268" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -4140,7 +4140,7 @@
         <v>656557</v>
       </c>
       <c r="C269" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -4151,7 +4151,7 @@
         <v>669713</v>
       </c>
       <c r="C270" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -4162,7 +4162,7 @@
         <v>663372</v>
       </c>
       <c r="C271" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="272" spans="1:3">
@@ -4173,7 +4173,7 @@
         <v>686249</v>
       </c>
       <c r="C272" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files for Aug 31
</commit_message>
<xml_diff>
--- a/assets/Historical_Starting_Pitchers.xlsx
+++ b/assets/Historical_Starting_Pitchers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="275">
   <si>
     <t>Baseball_Savant_Name</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Kodai Senga</t>
+  </si>
+  <si>
+    <t>Kyle Hart</t>
   </si>
   <si>
     <t>Lucas Giolito</t>
@@ -1193,7 +1196,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C272"/>
+  <dimension ref="A1:C273"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1218,7 +1221,7 @@
         <v>669467</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1229,7 +1232,7 @@
         <v>663903</v>
       </c>
       <c r="C3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1240,7 +1243,7 @@
         <v>694297</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1251,7 +1254,7 @@
         <v>605540</v>
       </c>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1262,7 +1265,7 @@
         <v>682243</v>
       </c>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1273,7 +1276,7 @@
         <v>686613</v>
       </c>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1284,7 +1287,7 @@
         <v>694462</v>
       </c>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1295,7 +1298,7 @@
         <v>669372</v>
       </c>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1306,7 +1309,7 @@
         <v>594798</v>
       </c>
       <c r="C10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1317,7 +1320,7 @@
         <v>666200</v>
       </c>
       <c r="C11" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1328,7 +1331,7 @@
         <v>657746</v>
       </c>
       <c r="C12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1339,7 +1342,7 @@
         <v>667755</v>
       </c>
       <c r="C13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1350,7 +1353,7 @@
         <v>434378</v>
       </c>
       <c r="C14" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1361,188 +1364,188 @@
         <v>673540</v>
       </c>
       <c r="C15" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>606996</v>
+      </c>
       <c r="C16" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>608337</v>
       </c>
       <c r="C17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>661563</v>
       </c>
       <c r="C18" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>527048</v>
       </c>
       <c r="C19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>571510</v>
       </c>
       <c r="C20" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>453286</v>
       </c>
       <c r="C21" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>608379</v>
       </c>
       <c r="C22" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>656605</v>
       </c>
       <c r="C23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>645261</v>
       </c>
       <c r="C24" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>676440</v>
       </c>
       <c r="C25" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>685299</v>
       </c>
       <c r="C26" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>669373</v>
       </c>
       <c r="C27" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>808967</v>
       </c>
       <c r="C28" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>608372</v>
       </c>
       <c r="C29" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>695418</v>
       </c>
       <c r="C30" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>693855</v>
       </c>
       <c r="C31" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32">
-        <v>671096</v>
-      </c>
       <c r="C32" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1550,10 +1553,10 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>519242</v>
+        <v>671096</v>
       </c>
       <c r="C33" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1561,10 +1564,10 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>650911</v>
+        <v>519242</v>
       </c>
       <c r="C34" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1572,10 +1575,10 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>656849</v>
+        <v>650911</v>
       </c>
       <c r="C35" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1583,10 +1586,10 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>669160</v>
+        <v>656849</v>
       </c>
       <c r="C36" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1594,7 +1597,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>593958</v>
+        <v>669160</v>
       </c>
       <c r="C37" t="s">
         <v>273</v>
@@ -1605,10 +1608,10 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>665795</v>
+        <v>593958</v>
       </c>
       <c r="C38" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1616,10 +1619,10 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>668909</v>
+        <v>665795</v>
       </c>
       <c r="C39" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1627,10 +1630,10 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>656427</v>
+        <v>668909</v>
       </c>
       <c r="C40" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1638,10 +1641,10 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>663623</v>
+        <v>656427</v>
       </c>
       <c r="C41" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1649,10 +1652,10 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>665871</v>
+        <v>663623</v>
       </c>
       <c r="C42" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1660,10 +1663,10 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>670912</v>
+        <v>665871</v>
       </c>
       <c r="C43" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1671,10 +1674,10 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>592332</v>
+        <v>670912</v>
       </c>
       <c r="C44" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1682,10 +1685,10 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>543294</v>
+        <v>592332</v>
       </c>
       <c r="C45" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1693,10 +1696,10 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>669302</v>
+        <v>543294</v>
       </c>
       <c r="C46" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1704,10 +1707,10 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>518876</v>
+        <v>669302</v>
       </c>
       <c r="C47" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1715,10 +1718,10 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>700241</v>
+        <v>518876</v>
       </c>
       <c r="C48" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1726,10 +1729,10 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>601713</v>
+        <v>700241</v>
       </c>
       <c r="C49" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1737,10 +1740,10 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>682990</v>
+        <v>601713</v>
       </c>
       <c r="C50" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1748,10 +1751,10 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>686752</v>
+        <v>682990</v>
       </c>
       <c r="C51" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1759,10 +1762,10 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>681293</v>
+        <v>686752</v>
       </c>
       <c r="C52" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1770,10 +1773,10 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>671737</v>
+        <v>681293</v>
       </c>
       <c r="C53" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1781,7 +1784,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>669432</v>
+        <v>671737</v>
       </c>
       <c r="C54" t="s">
         <v>273</v>
@@ -1792,10 +1795,10 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>607192</v>
+        <v>669432</v>
       </c>
       <c r="C55" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1803,10 +1806,10 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>681343</v>
+        <v>607192</v>
       </c>
       <c r="C56" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1814,10 +1817,10 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>663568</v>
+        <v>681343</v>
       </c>
       <c r="C57" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1825,10 +1828,10 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>693645</v>
+        <v>663568</v>
       </c>
       <c r="C58" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1836,10 +1839,10 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>693313</v>
+        <v>693645</v>
       </c>
       <c r="C59" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1847,10 +1850,10 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>685326</v>
+        <v>693313</v>
       </c>
       <c r="C60" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1858,10 +1861,10 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>686930</v>
+        <v>685326</v>
       </c>
       <c r="C61" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1869,10 +1872,10 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>605288</v>
+        <v>686930</v>
       </c>
       <c r="C62" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1880,7 +1883,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>605483</v>
+        <v>605288</v>
       </c>
       <c r="C63" t="s">
         <v>273</v>
@@ -1891,10 +1894,10 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>693821</v>
+        <v>605483</v>
       </c>
       <c r="C64" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1902,7 +1905,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>607074</v>
+        <v>693821</v>
       </c>
       <c r="C65" t="s">
         <v>273</v>
@@ -1913,10 +1916,10 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>663978</v>
+        <v>607074</v>
       </c>
       <c r="C66" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1924,10 +1927,10 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>664299</v>
+        <v>663978</v>
       </c>
       <c r="C67" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1935,10 +1938,10 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>665152</v>
+        <v>664299</v>
       </c>
       <c r="C68" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1946,10 +1949,10 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>691587</v>
+        <v>665152</v>
       </c>
       <c r="C69" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1957,10 +1960,10 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>642547</v>
+        <v>691587</v>
       </c>
       <c r="C70" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1968,10 +1971,10 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>669923</v>
+        <v>642547</v>
       </c>
       <c r="C71" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1979,10 +1982,10 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>608566</v>
+        <v>669923</v>
       </c>
       <c r="C72" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1990,10 +1993,10 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>683004</v>
+        <v>608566</v>
       </c>
       <c r="C73" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2001,7 +2004,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>605488</v>
+        <v>683004</v>
       </c>
       <c r="C74" t="s">
         <v>273</v>
@@ -2012,10 +2015,10 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>671106</v>
+        <v>605488</v>
       </c>
       <c r="C75" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2023,10 +2026,10 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>669461</v>
+        <v>671106</v>
       </c>
       <c r="C76" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2034,10 +2037,10 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>680730</v>
+        <v>669461</v>
       </c>
       <c r="C77" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2045,10 +2048,10 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>641482</v>
+        <v>680730</v>
       </c>
       <c r="C78" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2056,10 +2059,10 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>694973</v>
+        <v>641482</v>
       </c>
       <c r="C79" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2067,7 +2070,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>624133</v>
+        <v>694973</v>
       </c>
       <c r="C80" t="s">
         <v>273</v>
@@ -2078,10 +2081,10 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>592662</v>
+        <v>624133</v>
       </c>
       <c r="C81" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2089,10 +2092,10 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>607625</v>
+        <v>592662</v>
       </c>
       <c r="C82" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2100,10 +2103,10 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>669456</v>
+        <v>607625</v>
       </c>
       <c r="C83" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2111,7 +2114,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>542881</v>
+        <v>669456</v>
       </c>
       <c r="C84" t="s">
         <v>273</v>
@@ -2122,10 +2125,10 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>668678</v>
+        <v>542881</v>
       </c>
       <c r="C85" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2133,10 +2136,10 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>641793</v>
+        <v>668678</v>
       </c>
       <c r="C86" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2144,10 +2147,10 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>805673</v>
+        <v>641793</v>
       </c>
       <c r="C87" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2155,10 +2158,10 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>690990</v>
+        <v>805673</v>
       </c>
       <c r="C88" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2166,10 +2169,10 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>672782</v>
+        <v>690990</v>
       </c>
       <c r="C89" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2177,7 +2180,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>801139</v>
+        <v>672782</v>
       </c>
       <c r="C90" t="s">
         <v>273</v>
@@ -2188,10 +2191,10 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>804636</v>
+        <v>801139</v>
       </c>
       <c r="C91" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2199,10 +2202,10 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>605400</v>
+        <v>804636</v>
       </c>
       <c r="C92" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2210,10 +2213,10 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>800049</v>
+        <v>605400</v>
       </c>
       <c r="C93" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2221,7 +2224,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>700249</v>
+        <v>800049</v>
       </c>
       <c r="C94" t="s">
         <v>273</v>
@@ -2232,10 +2235,10 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>615698</v>
+        <v>700249</v>
       </c>
       <c r="C95" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2243,10 +2246,10 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>605280</v>
+        <v>615698</v>
       </c>
       <c r="C96" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2254,10 +2257,10 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>663436</v>
+        <v>605280</v>
       </c>
       <c r="C97" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2265,7 +2268,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>676979</v>
+        <v>663436</v>
       </c>
       <c r="C98" t="s">
         <v>273</v>
@@ -2276,10 +2279,10 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>500779</v>
+        <v>676979</v>
       </c>
       <c r="C99" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2287,10 +2290,10 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>607536</v>
+        <v>500779</v>
       </c>
       <c r="C100" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2298,10 +2301,10 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>657277</v>
+        <v>607536</v>
       </c>
       <c r="C101" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2309,10 +2312,10 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>571945</v>
+        <v>657277</v>
       </c>
       <c r="C102" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2320,10 +2323,10 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>622503</v>
+        <v>571945</v>
       </c>
       <c r="C103" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2331,7 +2334,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>684007</v>
+        <v>622503</v>
       </c>
       <c r="C104" t="s">
         <v>273</v>
@@ -2342,10 +2345,10 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>701542</v>
+        <v>684007</v>
       </c>
       <c r="C105" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2353,10 +2356,10 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>669920</v>
+        <v>701542</v>
       </c>
       <c r="C106" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2364,10 +2367,10 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>677952</v>
+        <v>669920</v>
       </c>
       <c r="C107" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2375,10 +2378,10 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>650644</v>
+        <v>677952</v>
       </c>
       <c r="C108" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2386,10 +2389,10 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>678394</v>
+        <v>650644</v>
       </c>
       <c r="C109" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2397,10 +2400,10 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>693433</v>
+        <v>678394</v>
       </c>
       <c r="C110" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2408,10 +2411,10 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>676917</v>
+        <v>693433</v>
       </c>
       <c r="C111" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2419,7 +2422,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>687931</v>
+        <v>676917</v>
       </c>
       <c r="C112" t="s">
         <v>273</v>
@@ -2430,10 +2433,10 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>663554</v>
+        <v>687931</v>
       </c>
       <c r="C113" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2441,10 +2444,10 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>607067</v>
+        <v>663554</v>
       </c>
       <c r="C114" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2452,10 +2455,10 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>656876</v>
+        <v>607067</v>
       </c>
       <c r="C115" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2463,7 +2466,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>641778</v>
+        <v>656876</v>
       </c>
       <c r="C116" t="s">
         <v>273</v>
@@ -2474,10 +2477,10 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>664285</v>
+        <v>641778</v>
       </c>
       <c r="C117" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2485,10 +2488,10 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>686799</v>
+        <v>664285</v>
       </c>
       <c r="C118" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2496,7 +2499,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>666214</v>
+        <v>686799</v>
       </c>
       <c r="C119" t="s">
         <v>273</v>
@@ -2507,10 +2510,10 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>608331</v>
+        <v>666214</v>
       </c>
       <c r="C120" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2518,10 +2521,10 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>666157</v>
+        <v>608331</v>
       </c>
       <c r="C121" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2529,10 +2532,10 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>672710</v>
+        <v>666157</v>
       </c>
       <c r="C122" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2540,10 +2543,10 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>669194</v>
+        <v>672710</v>
       </c>
       <c r="C123" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2551,10 +2554,10 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>660271</v>
+        <v>669194</v>
       </c>
       <c r="C124" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2562,10 +2565,10 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>680573</v>
+        <v>660271</v>
       </c>
       <c r="C125" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2573,10 +2576,10 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>677944</v>
+        <v>680573</v>
       </c>
       <c r="C126" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2584,10 +2587,10 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>543243</v>
+        <v>677944</v>
       </c>
       <c r="C127" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2595,10 +2598,10 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>592836</v>
+        <v>543243</v>
       </c>
       <c r="C128" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2606,10 +2609,10 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>506433</v>
+        <v>592836</v>
       </c>
       <c r="C129" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2617,10 +2620,10 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>801403</v>
+        <v>506433</v>
       </c>
       <c r="C130" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2628,10 +2631,10 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>687473</v>
+        <v>801403</v>
       </c>
       <c r="C131" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2639,10 +2642,10 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>686701</v>
+        <v>687473</v>
       </c>
       <c r="C132" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2650,7 +2653,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>656641</v>
+        <v>686701</v>
       </c>
       <c r="C133" t="s">
         <v>273</v>
@@ -2661,10 +2664,10 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>690997</v>
+        <v>656641</v>
       </c>
       <c r="C134" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2672,10 +2675,10 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>696149</v>
+        <v>690997</v>
       </c>
       <c r="C135" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2683,10 +2686,10 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>806960</v>
+        <v>696149</v>
       </c>
       <c r="C136" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2694,10 +2697,10 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>641927</v>
+        <v>806960</v>
       </c>
       <c r="C137" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2705,10 +2708,10 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>450203</v>
+        <v>641927</v>
       </c>
       <c r="C138" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2716,10 +2719,10 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>605135</v>
+        <v>450203</v>
       </c>
       <c r="C139" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2727,7 +2730,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>477132</v>
+        <v>605135</v>
       </c>
       <c r="C140" t="s">
         <v>273</v>
@@ -2738,10 +2741,10 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>656302</v>
+        <v>477132</v>
       </c>
       <c r="C141" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2749,10 +2752,10 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>680694</v>
+        <v>656302</v>
       </c>
       <c r="C142" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2760,10 +2763,10 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>622491</v>
+        <v>680694</v>
       </c>
       <c r="C143" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2771,7 +2774,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>669022</v>
+        <v>622491</v>
       </c>
       <c r="C144" t="s">
         <v>273</v>
@@ -2782,10 +2785,10 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>547179</v>
+        <v>669022</v>
       </c>
       <c r="C145" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2793,10 +2796,10 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>607259</v>
+        <v>547179</v>
       </c>
       <c r="C146" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2804,10 +2807,10 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>674370</v>
+        <v>607259</v>
       </c>
       <c r="C147" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2815,7 +2818,7 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>571578</v>
+        <v>674370</v>
       </c>
       <c r="C148" t="s">
         <v>273</v>
@@ -2826,10 +2829,10 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>640455</v>
+        <v>571578</v>
       </c>
       <c r="C149" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2837,10 +2840,10 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>669358</v>
+        <v>640455</v>
       </c>
       <c r="C150" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2848,7 +2851,7 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>579328</v>
+        <v>669358</v>
       </c>
       <c r="C151" t="s">
         <v>273</v>
@@ -2859,10 +2862,10 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>694819</v>
+        <v>579328</v>
       </c>
       <c r="C152" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2870,7 +2873,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>800048</v>
+        <v>694819</v>
       </c>
       <c r="C153" t="s">
         <v>273</v>
@@ -2881,10 +2884,10 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>686218</v>
+        <v>800048</v>
       </c>
       <c r="C154" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2892,10 +2895,10 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>668881</v>
+        <v>686218</v>
       </c>
       <c r="C155" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2903,7 +2906,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>676664</v>
+        <v>668881</v>
       </c>
       <c r="C156" t="s">
         <v>273</v>
@@ -2914,10 +2917,10 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>690916</v>
+        <v>676664</v>
       </c>
       <c r="C157" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2925,10 +2928,10 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>675911</v>
+        <v>690916</v>
       </c>
       <c r="C158" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2936,7 +2939,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>702070</v>
+        <v>675911</v>
       </c>
       <c r="C159" t="s">
         <v>273</v>
@@ -2947,10 +2950,10 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>592791</v>
+        <v>702070</v>
       </c>
       <c r="C160" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2958,7 +2961,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>688107</v>
+        <v>592791</v>
       </c>
       <c r="C161" t="s">
         <v>273</v>
@@ -2969,10 +2972,10 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>682052</v>
+        <v>688107</v>
       </c>
       <c r="C162" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2980,10 +2983,10 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>676083</v>
+        <v>682052</v>
       </c>
       <c r="C163" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2991,10 +2994,10 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>621244</v>
+        <v>676083</v>
       </c>
       <c r="C164" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3002,10 +3005,10 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>690953</v>
+        <v>621244</v>
       </c>
       <c r="C165" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3013,10 +3016,10 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>681347</v>
+        <v>690953</v>
       </c>
       <c r="C166" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3024,10 +3027,10 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>682929</v>
+        <v>681347</v>
       </c>
       <c r="C167" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3035,10 +3038,10 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>671212</v>
+        <v>682929</v>
       </c>
       <c r="C168" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3046,10 +3049,10 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>570632</v>
+        <v>671212</v>
       </c>
       <c r="C169" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3057,10 +3060,10 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>687064</v>
+        <v>570632</v>
       </c>
       <c r="C170" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3068,10 +3071,10 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>678022</v>
+        <v>687064</v>
       </c>
       <c r="C171" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3079,10 +3082,10 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>689017</v>
+        <v>678022</v>
       </c>
       <c r="C172" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3090,7 +3093,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>596295</v>
+        <v>689017</v>
       </c>
       <c r="C173" t="s">
         <v>273</v>
@@ -3098,21 +3101,21 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>154</v>
+        <v>174</v>
+      </c>
+      <c r="B174">
+        <v>596295</v>
       </c>
       <c r="C174" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>174</v>
-      </c>
-      <c r="B175">
-        <v>621111</v>
+        <v>155</v>
       </c>
       <c r="C175" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3120,10 +3123,10 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>694477</v>
+        <v>621111</v>
       </c>
       <c r="C176" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3131,10 +3134,10 @@
         <v>176</v>
       </c>
       <c r="B177">
-        <v>678906</v>
+        <v>694477</v>
       </c>
       <c r="C177" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3142,7 +3145,7 @@
         <v>177</v>
       </c>
       <c r="B178">
-        <v>571760</v>
+        <v>678906</v>
       </c>
       <c r="C178" t="s">
         <v>273</v>
@@ -3153,10 +3156,10 @@
         <v>178</v>
       </c>
       <c r="B179">
-        <v>607200</v>
+        <v>571760</v>
       </c>
       <c r="C179" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3164,10 +3167,10 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <v>543135</v>
+        <v>607200</v>
       </c>
       <c r="C180" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3175,10 +3178,10 @@
         <v>180</v>
       </c>
       <c r="B181">
-        <v>471911</v>
+        <v>543135</v>
       </c>
       <c r="C181" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3186,7 +3189,7 @@
         <v>181</v>
       </c>
       <c r="B182">
-        <v>663559</v>
+        <v>471911</v>
       </c>
       <c r="C182" t="s">
         <v>273</v>
@@ -3197,10 +3200,10 @@
         <v>182</v>
       </c>
       <c r="B183">
-        <v>647336</v>
+        <v>663559</v>
       </c>
       <c r="C183" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3208,10 +3211,10 @@
         <v>183</v>
       </c>
       <c r="B184">
-        <v>701519</v>
+        <v>647336</v>
       </c>
       <c r="C184" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3219,10 +3222,10 @@
         <v>184</v>
       </c>
       <c r="B185">
-        <v>677958</v>
+        <v>701519</v>
       </c>
       <c r="C185" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3230,10 +3233,10 @@
         <v>185</v>
       </c>
       <c r="B186">
-        <v>573186</v>
+        <v>677958</v>
       </c>
       <c r="C186" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3241,10 +3244,10 @@
         <v>186</v>
       </c>
       <c r="B187">
-        <v>686563</v>
+        <v>573186</v>
       </c>
       <c r="C187" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3252,10 +3255,10 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>622663</v>
+        <v>686563</v>
       </c>
       <c r="C188" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3263,7 +3266,7 @@
         <v>188</v>
       </c>
       <c r="B189">
-        <v>687922</v>
+        <v>622663</v>
       </c>
       <c r="C189" t="s">
         <v>273</v>
@@ -3274,10 +3277,10 @@
         <v>189</v>
       </c>
       <c r="B190">
-        <v>688138</v>
+        <v>687922</v>
       </c>
       <c r="C190" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3285,10 +3288,10 @@
         <v>190</v>
       </c>
       <c r="B191">
-        <v>701487</v>
+        <v>688138</v>
       </c>
       <c r="C191" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3296,10 +3299,10 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>687134</v>
+        <v>701487</v>
       </c>
       <c r="C192" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3307,10 +3310,10 @@
         <v>192</v>
       </c>
       <c r="B193">
-        <v>593423</v>
+        <v>687134</v>
       </c>
       <c r="C193" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3318,7 +3321,7 @@
         <v>193</v>
       </c>
       <c r="B194">
-        <v>448179</v>
+        <v>593423</v>
       </c>
       <c r="C194" t="s">
         <v>273</v>
@@ -3329,10 +3332,10 @@
         <v>194</v>
       </c>
       <c r="B195">
-        <v>621107</v>
+        <v>448179</v>
       </c>
       <c r="C195" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3340,10 +3343,10 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>695505</v>
+        <v>621107</v>
       </c>
       <c r="C196" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3351,10 +3354,10 @@
         <v>196</v>
       </c>
       <c r="B197">
-        <v>675512</v>
+        <v>695505</v>
       </c>
       <c r="C197" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3362,10 +3365,10 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>676962</v>
+        <v>675512</v>
       </c>
       <c r="C198" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3373,7 +3376,7 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>676282</v>
+        <v>676962</v>
       </c>
       <c r="C199" t="s">
         <v>273</v>
@@ -3384,10 +3387,10 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>680732</v>
+        <v>676282</v>
       </c>
       <c r="C200" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3395,10 +3398,10 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>554430</v>
+        <v>680732</v>
       </c>
       <c r="C201" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3406,7 +3409,7 @@
         <v>201</v>
       </c>
       <c r="B202">
-        <v>676467</v>
+        <v>554430</v>
       </c>
       <c r="C202" t="s">
         <v>273</v>
@@ -3417,10 +3420,10 @@
         <v>202</v>
       </c>
       <c r="B203">
-        <v>656550</v>
+        <v>676467</v>
       </c>
       <c r="C203" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3428,7 +3431,7 @@
         <v>203</v>
       </c>
       <c r="B204">
-        <v>663460</v>
+        <v>656550</v>
       </c>
       <c r="C204" t="s">
         <v>273</v>
@@ -3439,10 +3442,10 @@
         <v>204</v>
       </c>
       <c r="B205">
-        <v>681190</v>
+        <v>663460</v>
       </c>
       <c r="C205" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3450,10 +3453,10 @@
         <v>205</v>
       </c>
       <c r="B206">
-        <v>669721</v>
+        <v>681190</v>
       </c>
       <c r="C206" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3461,10 +3464,10 @@
         <v>206</v>
       </c>
       <c r="B207">
-        <v>701581</v>
+        <v>669721</v>
       </c>
       <c r="C207" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3472,10 +3475,10 @@
         <v>207</v>
       </c>
       <c r="B208">
-        <v>806185</v>
+        <v>701581</v>
       </c>
       <c r="C208" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3483,10 +3486,10 @@
         <v>208</v>
       </c>
       <c r="B209">
-        <v>672456</v>
+        <v>806185</v>
       </c>
       <c r="C209" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3494,7 +3497,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>687888</v>
+        <v>672456</v>
       </c>
       <c r="C210" t="s">
         <v>273</v>
@@ -3505,10 +3508,10 @@
         <v>210</v>
       </c>
       <c r="B211">
-        <v>681857</v>
+        <v>687888</v>
       </c>
       <c r="C211" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3516,10 +3519,10 @@
         <v>211</v>
       </c>
       <c r="B212">
-        <v>666171</v>
+        <v>681857</v>
       </c>
       <c r="C212" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3527,10 +3530,10 @@
         <v>212</v>
       </c>
       <c r="B213">
-        <v>663795</v>
+        <v>666171</v>
       </c>
       <c r="C213" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3538,7 +3541,7 @@
         <v>213</v>
       </c>
       <c r="B214">
-        <v>696136</v>
+        <v>663795</v>
       </c>
       <c r="C214" t="s">
         <v>273</v>
@@ -3549,10 +3552,10 @@
         <v>214</v>
       </c>
       <c r="B215">
-        <v>680736</v>
+        <v>696136</v>
       </c>
       <c r="C215" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3560,10 +3563,10 @@
         <v>215</v>
       </c>
       <c r="B216">
-        <v>642216</v>
+        <v>680736</v>
       </c>
       <c r="C216" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3571,10 +3574,10 @@
         <v>216</v>
       </c>
       <c r="B217">
-        <v>621112</v>
+        <v>642216</v>
       </c>
       <c r="C217" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3582,10 +3585,10 @@
         <v>217</v>
       </c>
       <c r="B218">
-        <v>680885</v>
+        <v>621112</v>
       </c>
       <c r="C218" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3593,10 +3596,10 @@
         <v>218</v>
       </c>
       <c r="B219">
-        <v>605513</v>
+        <v>680885</v>
       </c>
       <c r="C219" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3604,7 +3607,7 @@
         <v>219</v>
       </c>
       <c r="B220">
-        <v>641302</v>
+        <v>605513</v>
       </c>
       <c r="C220" t="s">
         <v>273</v>
@@ -3615,10 +3618,10 @@
         <v>220</v>
       </c>
       <c r="B221">
-        <v>690928</v>
+        <v>641302</v>
       </c>
       <c r="C221" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3626,10 +3629,10 @@
         <v>221</v>
       </c>
       <c r="B222">
-        <v>694918</v>
+        <v>690928</v>
       </c>
       <c r="C222" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3637,10 +3640,10 @@
         <v>222</v>
       </c>
       <c r="B223">
-        <v>800311</v>
+        <v>694918</v>
       </c>
       <c r="C223" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3648,10 +3651,10 @@
         <v>223</v>
       </c>
       <c r="B224">
-        <v>592866</v>
+        <v>800311</v>
       </c>
       <c r="C224" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3659,10 +3662,10 @@
         <v>224</v>
       </c>
       <c r="B225">
-        <v>678024</v>
+        <v>592866</v>
       </c>
       <c r="C225" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3670,7 +3673,7 @@
         <v>225</v>
       </c>
       <c r="B226">
-        <v>642232</v>
+        <v>678024</v>
       </c>
       <c r="C226" t="s">
         <v>273</v>
@@ -3681,10 +3684,10 @@
         <v>226</v>
       </c>
       <c r="B227">
-        <v>669422</v>
+        <v>642232</v>
       </c>
       <c r="C227" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3692,10 +3695,10 @@
         <v>227</v>
       </c>
       <c r="B228">
-        <v>657376</v>
+        <v>669422</v>
       </c>
       <c r="C228" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3703,10 +3706,10 @@
         <v>228</v>
       </c>
       <c r="B229">
-        <v>676508</v>
+        <v>657376</v>
       </c>
       <c r="C229" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3714,7 +3717,7 @@
         <v>229</v>
       </c>
       <c r="B230">
-        <v>687223</v>
+        <v>676508</v>
       </c>
       <c r="C230" t="s">
         <v>273</v>
@@ -3725,10 +3728,10 @@
         <v>230</v>
       </c>
       <c r="B231">
-        <v>656288</v>
+        <v>687223</v>
       </c>
       <c r="C231" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3736,7 +3739,7 @@
         <v>231</v>
       </c>
       <c r="B232">
-        <v>690986</v>
+        <v>656288</v>
       </c>
       <c r="C232" t="s">
         <v>273</v>
@@ -3747,10 +3750,10 @@
         <v>232</v>
       </c>
       <c r="B233">
-        <v>687765</v>
+        <v>690986</v>
       </c>
       <c r="C233" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3758,10 +3761,10 @@
         <v>233</v>
       </c>
       <c r="B234">
-        <v>641816</v>
+        <v>687765</v>
       </c>
       <c r="C234" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3769,10 +3772,10 @@
         <v>234</v>
       </c>
       <c r="B235">
-        <v>687830</v>
+        <v>641816</v>
       </c>
       <c r="C235" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3780,27 +3783,27 @@
         <v>235</v>
       </c>
       <c r="B236">
-        <v>676106</v>
+        <v>687830</v>
       </c>
       <c r="C236" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
         <v>236</v>
       </c>
+      <c r="B237">
+        <v>676106</v>
+      </c>
       <c r="C237" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
         <v>237</v>
       </c>
-      <c r="B238">
-        <v>489119</v>
-      </c>
       <c r="C238" t="s">
         <v>273</v>
       </c>
@@ -3810,29 +3813,29 @@
         <v>238</v>
       </c>
       <c r="B239">
-        <v>670102</v>
+        <v>489119</v>
       </c>
       <c r="C239" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
         <v>239</v>
       </c>
+      <c r="B240">
+        <v>670102</v>
+      </c>
       <c r="C240" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
         <v>240</v>
       </c>
-      <c r="B241">
-        <v>656731</v>
-      </c>
       <c r="C241" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3840,10 +3843,10 @@
         <v>241</v>
       </c>
       <c r="B242">
-        <v>676961</v>
+        <v>656731</v>
       </c>
       <c r="C242" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3851,7 +3854,7 @@
         <v>242</v>
       </c>
       <c r="B243">
-        <v>677960</v>
+        <v>676961</v>
       </c>
       <c r="C243" t="s">
         <v>273</v>
@@ -3862,10 +3865,10 @@
         <v>243</v>
       </c>
       <c r="B244">
-        <v>605452</v>
+        <v>677960</v>
       </c>
       <c r="C244" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3873,7 +3876,7 @@
         <v>244</v>
       </c>
       <c r="B245">
-        <v>666142</v>
+        <v>605452</v>
       </c>
       <c r="C245" t="s">
         <v>273</v>
@@ -3884,10 +3887,10 @@
         <v>245</v>
       </c>
       <c r="B246">
-        <v>689017</v>
+        <v>666142</v>
       </c>
       <c r="C246" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3895,10 +3898,10 @@
         <v>246</v>
       </c>
       <c r="B247">
-        <v>664062</v>
+        <v>689017</v>
       </c>
       <c r="C247" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3906,7 +3909,7 @@
         <v>247</v>
       </c>
       <c r="B248">
-        <v>676428</v>
+        <v>664062</v>
       </c>
       <c r="C248" t="s">
         <v>273</v>
@@ -3917,10 +3920,10 @@
         <v>248</v>
       </c>
       <c r="B249">
-        <v>641154</v>
+        <v>676428</v>
       </c>
       <c r="C249" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3928,10 +3931,10 @@
         <v>249</v>
       </c>
       <c r="B250">
-        <v>676974</v>
+        <v>641154</v>
       </c>
       <c r="C250" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3939,10 +3942,10 @@
         <v>250</v>
       </c>
       <c r="B251">
-        <v>669203</v>
+        <v>676974</v>
       </c>
       <c r="C251" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3950,10 +3953,10 @@
         <v>251</v>
       </c>
       <c r="B252">
-        <v>680684</v>
+        <v>669203</v>
       </c>
       <c r="C252" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3961,10 +3964,10 @@
         <v>252</v>
       </c>
       <c r="B253">
-        <v>700363</v>
+        <v>680684</v>
       </c>
       <c r="C253" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -3972,7 +3975,7 @@
         <v>253</v>
       </c>
       <c r="B254">
-        <v>663465</v>
+        <v>700363</v>
       </c>
       <c r="C254" t="s">
         <v>273</v>
@@ -3983,10 +3986,10 @@
         <v>254</v>
       </c>
       <c r="B255">
-        <v>695549</v>
+        <v>663465</v>
       </c>
       <c r="C255" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -3994,7 +3997,7 @@
         <v>255</v>
       </c>
       <c r="B256">
-        <v>663738</v>
+        <v>695549</v>
       </c>
       <c r="C256" t="s">
         <v>273</v>
@@ -4005,10 +4008,10 @@
         <v>256</v>
       </c>
       <c r="B257">
-        <v>701656</v>
+        <v>663738</v>
       </c>
       <c r="C257" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -4016,10 +4019,10 @@
         <v>257</v>
       </c>
       <c r="B258">
-        <v>650633</v>
+        <v>701656</v>
       </c>
       <c r="C258" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -4027,10 +4030,10 @@
         <v>258</v>
       </c>
       <c r="B259">
-        <v>694646</v>
+        <v>650633</v>
       </c>
       <c r="C259" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -4038,10 +4041,10 @@
         <v>259</v>
       </c>
       <c r="B260">
-        <v>669060</v>
+        <v>694646</v>
       </c>
       <c r="C260" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -4049,10 +4052,10 @@
         <v>260</v>
       </c>
       <c r="B261">
-        <v>669387</v>
+        <v>669060</v>
       </c>
       <c r="C261" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -4060,10 +4063,10 @@
         <v>261</v>
       </c>
       <c r="B262">
-        <v>502043</v>
+        <v>669387</v>
       </c>
       <c r="C262" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -4071,10 +4074,10 @@
         <v>262</v>
       </c>
       <c r="B263">
-        <v>669854</v>
+        <v>502043</v>
       </c>
       <c r="C263" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -4082,10 +4085,10 @@
         <v>263</v>
       </c>
       <c r="B264">
-        <v>668964</v>
+        <v>669854</v>
       </c>
       <c r="C264" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -4093,10 +4096,10 @@
         <v>264</v>
       </c>
       <c r="B265">
-        <v>695534</v>
+        <v>668964</v>
       </c>
       <c r="C265" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -4104,10 +4107,10 @@
         <v>265</v>
       </c>
       <c r="B266">
-        <v>663855</v>
+        <v>695534</v>
       </c>
       <c r="C266" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -4115,10 +4118,10 @@
         <v>266</v>
       </c>
       <c r="B267">
-        <v>678368</v>
+        <v>663855</v>
       </c>
       <c r="C267" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -4126,10 +4129,10 @@
         <v>267</v>
       </c>
       <c r="B268">
-        <v>594902</v>
+        <v>678368</v>
       </c>
       <c r="C268" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -4137,10 +4140,10 @@
         <v>268</v>
       </c>
       <c r="B269">
-        <v>656557</v>
+        <v>594902</v>
       </c>
       <c r="C269" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -4148,10 +4151,10 @@
         <v>269</v>
       </c>
       <c r="B270">
-        <v>669713</v>
+        <v>656557</v>
       </c>
       <c r="C270" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -4159,10 +4162,10 @@
         <v>270</v>
       </c>
       <c r="B271">
-        <v>663372</v>
+        <v>669713</v>
       </c>
       <c r="C271" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="272" spans="1:3">
@@ -4170,10 +4173,21 @@
         <v>271</v>
       </c>
       <c r="B272">
+        <v>663372</v>
+      </c>
+      <c r="C272" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" t="s">
+        <v>272</v>
+      </c>
+      <c r="B273">
         <v>686249</v>
       </c>
-      <c r="C272" t="s">
-        <v>272</v>
+      <c r="C273" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding data for Sept 1
</commit_message>
<xml_diff>
--- a/assets/Historical_Starting_Pitchers.xlsx
+++ b/assets/Historical_Starting_Pitchers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="277">
   <si>
     <t>Baseball_Savant_Name</t>
   </si>
@@ -25,6 +25,81 @@
     <t>Handedness</t>
   </si>
   <si>
+    <t>Bailey Ober</t>
+  </si>
+  <si>
+    <t>Brayan Bello</t>
+  </si>
+  <si>
+    <t>Bryse Wilson</t>
+  </si>
+  <si>
+    <t>Charlie Morton</t>
+  </si>
+  <si>
+    <t>Chris Bassitt</t>
+  </si>
+  <si>
+    <t>Colin Rea</t>
+  </si>
+  <si>
+    <t>Dylan Cease</t>
+  </si>
+  <si>
+    <t>Hunter Greene</t>
+  </si>
+  <si>
+    <t>Kyle Bradish</t>
+  </si>
+  <si>
+    <t>Luis Castillo</t>
+  </si>
+  <si>
+    <t>Patrick Corbin</t>
+  </si>
+  <si>
+    <t>Ryne Nelson</t>
+  </si>
+  <si>
+    <t>Sean Manaea</t>
+  </si>
+  <si>
+    <t>Shane Baz</t>
+  </si>
+  <si>
+    <t>Sonny Gray</t>
+  </si>
+  <si>
+    <t>Spencer Strider</t>
+  </si>
+  <si>
+    <t>Taijuan Walker</t>
+  </si>
+  <si>
+    <t>Yusei Kikuchi</t>
+  </si>
+  <si>
+    <t>Chase Dollander</t>
+  </si>
+  <si>
+    <t>Jacob Misiorowski</t>
+  </si>
+  <si>
+    <t>Kai-Wei Teng</t>
+  </si>
+  <si>
+    <t>Parker Messick</t>
+  </si>
+  <si>
+    <t>Luis Morales</t>
+  </si>
+  <si>
+    <t>Luarbert Arias</t>
+  </si>
+  <si>
+    <t>Andrew Alvarez</t>
+  </si>
+  <si>
     <t>Andre Pallante</t>
   </si>
   <si>
@@ -346,9 +421,6 @@
     <t>Aaron Civale</t>
   </si>
   <si>
-    <t>Brayan Bello</t>
-  </si>
-  <si>
     <t>Bryan Woo</t>
   </si>
   <si>
@@ -361,9 +433,6 @@
     <t>Casey Mize</t>
   </si>
   <si>
-    <t>Colin Rea</t>
-  </si>
-  <si>
     <t>Drew Rasmussen</t>
   </si>
   <si>
@@ -388,9 +457,6 @@
     <t>Roansy Contreras</t>
   </si>
   <si>
-    <t>Ryne Nelson</t>
-  </si>
-  <si>
     <t>Shohei Ohtani</t>
   </si>
   <si>
@@ -400,18 +466,9 @@
     <t>Slade Cecconi</t>
   </si>
   <si>
-    <t>Sonny Gray</t>
-  </si>
-  <si>
-    <t>Taijuan Walker</t>
-  </si>
-  <si>
     <t>Yu Darvish</t>
   </si>
   <si>
-    <t>Chase Dollander</t>
-  </si>
-  <si>
     <t>Ryan Gusto</t>
   </si>
   <si>
@@ -427,30 +484,9 @@
     <t>Bubba Chandler</t>
   </si>
   <si>
-    <t>Luis Morales</t>
-  </si>
-  <si>
-    <t>Bailey Ober</t>
-  </si>
-  <si>
-    <t>Charlie Morton</t>
-  </si>
-  <si>
-    <t>Chris Bassitt</t>
-  </si>
-  <si>
     <t>Clayton Kershaw</t>
   </si>
   <si>
-    <t>Dylan Cease</t>
-  </si>
-  <si>
-    <t>Kyle Bradish</t>
-  </si>
-  <si>
-    <t>Luis Castillo</t>
-  </si>
-  <si>
     <t>MacKenzie Gore</t>
   </si>
   <si>
@@ -463,39 +499,15 @@
     <t>Osvaldo Bido</t>
   </si>
   <si>
-    <t>Patrick Corbin</t>
-  </si>
-  <si>
-    <t>Sean Manaea</t>
-  </si>
-  <si>
-    <t>Shane Baz</t>
-  </si>
-  <si>
-    <t>Yusei Kikuchi</t>
-  </si>
-  <si>
-    <t>Jacob Misiorowski</t>
-  </si>
-  <si>
-    <t>Parker Messick</t>
-  </si>
-  <si>
     <t>Emmet Sheehan</t>
   </si>
   <si>
-    <t>Hunter Greene</t>
-  </si>
-  <si>
     <t>JP Sears</t>
   </si>
   <si>
     <t>Richard Fitts</t>
   </si>
   <si>
-    <t>Spencer Strider</t>
-  </si>
-  <si>
     <t>Noah Cameron</t>
   </si>
   <si>
@@ -547,9 +559,6 @@
     <t>Chad Patrick</t>
   </si>
   <si>
-    <t>Kai-Wei Teng</t>
-  </si>
-  <si>
     <t>Andrew Heaney</t>
   </si>
   <si>
@@ -794,9 +803,6 @@
   </si>
   <si>
     <t>Chayce McDermott</t>
-  </si>
-  <si>
-    <t>Bryse Wilson</t>
   </si>
   <si>
     <t>Carmen Mlodzinski</t>
@@ -1196,7 +1202,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C273"/>
+  <dimension ref="A1:C275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1218,10 +1224,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>669467</v>
+        <v>641927</v>
       </c>
       <c r="C2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1229,10 +1235,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>663903</v>
+        <v>678394</v>
       </c>
       <c r="C3" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1240,10 +1246,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>694297</v>
+        <v>669060</v>
       </c>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1251,10 +1257,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>605540</v>
+        <v>450203</v>
       </c>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1262,10 +1268,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>682243</v>
+        <v>605135</v>
       </c>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1273,10 +1279,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>686613</v>
+        <v>607067</v>
       </c>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1284,10 +1290,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>694462</v>
+        <v>656302</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1295,10 +1301,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>669372</v>
+        <v>668881</v>
       </c>
       <c r="C9" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1306,10 +1312,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>594798</v>
+        <v>680694</v>
       </c>
       <c r="C10" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1317,235 +1323,235 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>666200</v>
+        <v>622491</v>
       </c>
       <c r="C11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>657746</v>
-      </c>
       <c r="C12" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>667755</v>
+        <v>571578</v>
       </c>
       <c r="C13" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>434378</v>
+        <v>669194</v>
       </c>
       <c r="C14" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>673540</v>
+        <v>640455</v>
       </c>
       <c r="C15" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>606996</v>
+        <v>669358</v>
       </c>
       <c r="C16" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>608337</v>
+        <v>543243</v>
       </c>
       <c r="C17" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>661563</v>
+        <v>675911</v>
       </c>
       <c r="C18" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>527048</v>
+        <v>592836</v>
       </c>
       <c r="C19" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>571510</v>
+        <v>579328</v>
       </c>
       <c r="C20" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>453286</v>
+        <v>801403</v>
       </c>
       <c r="C21" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
-        <v>608379</v>
+        <v>694819</v>
       </c>
       <c r="C22" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>656605</v>
+        <v>678906</v>
       </c>
       <c r="C23" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>645261</v>
+        <v>800048</v>
       </c>
       <c r="C24" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>676440</v>
+        <v>806960</v>
       </c>
       <c r="C25" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>685299</v>
+        <v>678215</v>
       </c>
       <c r="C26" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>669373</v>
+        <v>674841</v>
       </c>
       <c r="C27" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>808967</v>
+        <v>669467</v>
       </c>
       <c r="C28" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>608372</v>
+        <v>663903</v>
       </c>
       <c r="C29" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30">
-        <v>695418</v>
+        <v>694297</v>
       </c>
       <c r="C30" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>605540</v>
+      </c>
+      <c r="C31" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B31">
-        <v>693855</v>
-      </c>
-      <c r="C31" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="B32">
+        <v>682243</v>
+      </c>
       <c r="C32" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1553,10 +1559,10 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>671096</v>
+        <v>686613</v>
       </c>
       <c r="C33" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1564,10 +1570,10 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>519242</v>
+        <v>694462</v>
       </c>
       <c r="C34" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1575,10 +1581,10 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>650911</v>
+        <v>669372</v>
       </c>
       <c r="C35" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1586,10 +1592,10 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>656849</v>
+        <v>594798</v>
       </c>
       <c r="C36" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1597,10 +1603,10 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>669160</v>
+        <v>666200</v>
       </c>
       <c r="C37" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1608,10 +1614,10 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>593958</v>
+        <v>657746</v>
       </c>
       <c r="C38" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1619,10 +1625,10 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>665795</v>
+        <v>667755</v>
       </c>
       <c r="C39" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1630,10 +1636,10 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>668909</v>
+        <v>434378</v>
       </c>
       <c r="C40" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1641,10 +1647,10 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>656427</v>
+        <v>673540</v>
       </c>
       <c r="C41" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1652,10 +1658,10 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>663623</v>
+        <v>606996</v>
       </c>
       <c r="C42" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1663,10 +1669,10 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>665871</v>
+        <v>608337</v>
       </c>
       <c r="C43" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1674,10 +1680,10 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>670912</v>
+        <v>661563</v>
       </c>
       <c r="C44" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1685,10 +1691,10 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>592332</v>
+        <v>527048</v>
       </c>
       <c r="C45" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1696,10 +1702,10 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>543294</v>
+        <v>571510</v>
       </c>
       <c r="C46" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1707,10 +1713,10 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>669302</v>
+        <v>453286</v>
       </c>
       <c r="C47" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1718,10 +1724,10 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>518876</v>
+        <v>608379</v>
       </c>
       <c r="C48" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1729,10 +1735,10 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>700241</v>
+        <v>656605</v>
       </c>
       <c r="C49" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1740,10 +1746,10 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>601713</v>
+        <v>645261</v>
       </c>
       <c r="C50" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1751,10 +1757,10 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>682990</v>
+        <v>676440</v>
       </c>
       <c r="C51" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1762,10 +1768,10 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>686752</v>
+        <v>685299</v>
       </c>
       <c r="C52" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1773,10 +1779,10 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>681293</v>
+        <v>669373</v>
       </c>
       <c r="C53" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1784,10 +1790,10 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>671737</v>
+        <v>808967</v>
       </c>
       <c r="C54" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1795,10 +1801,10 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>669432</v>
+        <v>608372</v>
       </c>
       <c r="C55" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1806,10 +1812,10 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>607192</v>
+        <v>695418</v>
       </c>
       <c r="C56" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1817,10 +1823,10 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>681343</v>
+        <v>693855</v>
       </c>
       <c r="C57" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1828,10 +1834,10 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>663568</v>
+        <v>671096</v>
       </c>
       <c r="C58" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1839,10 +1845,10 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>693645</v>
+        <v>519242</v>
       </c>
       <c r="C59" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1850,10 +1856,10 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>693313</v>
+        <v>650911</v>
       </c>
       <c r="C60" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1861,10 +1867,10 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>685326</v>
+        <v>656849</v>
       </c>
       <c r="C61" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1872,10 +1878,10 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>686930</v>
+        <v>669160</v>
       </c>
       <c r="C62" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1883,10 +1889,10 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>605288</v>
+        <v>593958</v>
       </c>
       <c r="C63" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1894,10 +1900,10 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>605483</v>
+        <v>665795</v>
       </c>
       <c r="C64" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1905,10 +1911,10 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>693821</v>
+        <v>668909</v>
       </c>
       <c r="C65" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1916,10 +1922,10 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>607074</v>
+        <v>656427</v>
       </c>
       <c r="C66" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1927,10 +1933,10 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>663978</v>
+        <v>663623</v>
       </c>
       <c r="C67" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1938,10 +1944,10 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>664299</v>
+        <v>665871</v>
       </c>
       <c r="C68" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1949,10 +1955,10 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>665152</v>
+        <v>670912</v>
       </c>
       <c r="C69" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1960,10 +1966,10 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>691587</v>
+        <v>592332</v>
       </c>
       <c r="C70" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1971,10 +1977,10 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>642547</v>
+        <v>543294</v>
       </c>
       <c r="C71" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1982,10 +1988,10 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>669923</v>
+        <v>669302</v>
       </c>
       <c r="C72" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1993,10 +1999,10 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>608566</v>
+        <v>518876</v>
       </c>
       <c r="C73" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2004,10 +2010,10 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>683004</v>
+        <v>700241</v>
       </c>
       <c r="C74" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2015,10 +2021,10 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>605488</v>
+        <v>601713</v>
       </c>
       <c r="C75" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2026,10 +2032,10 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>671106</v>
+        <v>682990</v>
       </c>
       <c r="C76" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2037,10 +2043,10 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>669461</v>
+        <v>686752</v>
       </c>
       <c r="C77" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2048,10 +2054,10 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>680730</v>
+        <v>681293</v>
       </c>
       <c r="C78" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2059,10 +2065,10 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>641482</v>
+        <v>671737</v>
       </c>
       <c r="C79" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2070,10 +2076,10 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>694973</v>
+        <v>669432</v>
       </c>
       <c r="C80" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2081,10 +2087,10 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>624133</v>
+        <v>607192</v>
       </c>
       <c r="C81" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2092,10 +2098,10 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>592662</v>
+        <v>681343</v>
       </c>
       <c r="C82" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2103,10 +2109,10 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>607625</v>
+        <v>663568</v>
       </c>
       <c r="C83" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2114,10 +2120,10 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>669456</v>
+        <v>693645</v>
       </c>
       <c r="C84" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2125,10 +2131,10 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>542881</v>
+        <v>693313</v>
       </c>
       <c r="C85" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2136,10 +2142,10 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>668678</v>
+        <v>685326</v>
       </c>
       <c r="C86" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2147,10 +2153,10 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>641793</v>
+        <v>686930</v>
       </c>
       <c r="C87" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2158,10 +2164,10 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>805673</v>
+        <v>605288</v>
       </c>
       <c r="C88" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2169,10 +2175,10 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>690990</v>
+        <v>605483</v>
       </c>
       <c r="C89" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2180,10 +2186,10 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>672782</v>
+        <v>693821</v>
       </c>
       <c r="C90" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2191,10 +2197,10 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>801139</v>
+        <v>607074</v>
       </c>
       <c r="C91" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2202,10 +2208,10 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>804636</v>
+        <v>663978</v>
       </c>
       <c r="C92" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2213,10 +2219,10 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>605400</v>
+        <v>664299</v>
       </c>
       <c r="C93" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2224,10 +2230,10 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>800049</v>
+        <v>665152</v>
       </c>
       <c r="C94" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2235,10 +2241,10 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>700249</v>
+        <v>691587</v>
       </c>
       <c r="C95" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2246,10 +2252,10 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>615698</v>
+        <v>642547</v>
       </c>
       <c r="C96" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2257,10 +2263,10 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>605280</v>
+        <v>669923</v>
       </c>
       <c r="C97" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2268,10 +2274,10 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>663436</v>
+        <v>608566</v>
       </c>
       <c r="C98" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2279,10 +2285,10 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>676979</v>
+        <v>683004</v>
       </c>
       <c r="C99" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2290,10 +2296,10 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>500779</v>
+        <v>605488</v>
       </c>
       <c r="C100" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2301,10 +2307,10 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>607536</v>
+        <v>671106</v>
       </c>
       <c r="C101" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2312,10 +2318,10 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>657277</v>
+        <v>669461</v>
       </c>
       <c r="C102" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2323,10 +2329,10 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>571945</v>
+        <v>680730</v>
       </c>
       <c r="C103" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2334,10 +2340,10 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>622503</v>
+        <v>641482</v>
       </c>
       <c r="C104" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2345,10 +2351,10 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>684007</v>
+        <v>694973</v>
       </c>
       <c r="C105" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2356,10 +2362,10 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>701542</v>
+        <v>624133</v>
       </c>
       <c r="C106" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2367,10 +2373,10 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>669920</v>
+        <v>592662</v>
       </c>
       <c r="C107" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2378,10 +2384,10 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>677952</v>
+        <v>607625</v>
       </c>
       <c r="C108" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2389,10 +2395,10 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>650644</v>
+        <v>669456</v>
       </c>
       <c r="C109" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2400,10 +2406,10 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>678394</v>
+        <v>542881</v>
       </c>
       <c r="C110" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2411,10 +2417,10 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>693433</v>
+        <v>668678</v>
       </c>
       <c r="C111" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2422,10 +2428,10 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>676917</v>
+        <v>641793</v>
       </c>
       <c r="C112" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2433,10 +2439,10 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>687931</v>
+        <v>805673</v>
       </c>
       <c r="C113" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2444,10 +2450,10 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>663554</v>
+        <v>690990</v>
       </c>
       <c r="C114" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2455,10 +2461,10 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>607067</v>
+        <v>672782</v>
       </c>
       <c r="C115" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2466,10 +2472,10 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>656876</v>
+        <v>801139</v>
       </c>
       <c r="C116" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2477,10 +2483,10 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>641778</v>
+        <v>804636</v>
       </c>
       <c r="C117" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2488,10 +2494,10 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>664285</v>
+        <v>605400</v>
       </c>
       <c r="C118" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2499,10 +2505,10 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>686799</v>
+        <v>800049</v>
       </c>
       <c r="C119" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2510,10 +2516,10 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>666214</v>
+        <v>700249</v>
       </c>
       <c r="C120" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2521,10 +2527,10 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>608331</v>
+        <v>615698</v>
       </c>
       <c r="C121" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2532,10 +2538,10 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>666157</v>
+        <v>605280</v>
       </c>
       <c r="C122" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2543,10 +2549,10 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>672710</v>
+        <v>663436</v>
       </c>
       <c r="C123" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2554,10 +2560,10 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>669194</v>
+        <v>676979</v>
       </c>
       <c r="C124" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2565,10 +2571,10 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>660271</v>
+        <v>500779</v>
       </c>
       <c r="C125" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2576,10 +2582,10 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>680573</v>
+        <v>607536</v>
       </c>
       <c r="C126" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2587,10 +2593,10 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>677944</v>
+        <v>657277</v>
       </c>
       <c r="C127" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2598,10 +2604,10 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>543243</v>
+        <v>571945</v>
       </c>
       <c r="C128" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2609,10 +2615,10 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>592836</v>
+        <v>622503</v>
       </c>
       <c r="C129" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2620,10 +2626,10 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>506433</v>
+        <v>684007</v>
       </c>
       <c r="C130" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2631,10 +2637,10 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>801403</v>
+        <v>701542</v>
       </c>
       <c r="C131" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2642,10 +2648,10 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>687473</v>
+        <v>669920</v>
       </c>
       <c r="C132" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2653,10 +2659,10 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>686701</v>
+        <v>677952</v>
       </c>
       <c r="C133" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2664,10 +2670,10 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>656641</v>
+        <v>650644</v>
       </c>
       <c r="C134" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2675,10 +2681,10 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>690997</v>
+        <v>693433</v>
       </c>
       <c r="C135" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2686,10 +2692,10 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>696149</v>
+        <v>676917</v>
       </c>
       <c r="C136" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2697,10 +2703,10 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>806960</v>
+        <v>687931</v>
       </c>
       <c r="C137" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2708,10 +2714,10 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>641927</v>
+        <v>663554</v>
       </c>
       <c r="C138" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2719,10 +2725,10 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>450203</v>
+        <v>656876</v>
       </c>
       <c r="C139" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2730,10 +2736,10 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>605135</v>
+        <v>641778</v>
       </c>
       <c r="C140" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2741,10 +2747,10 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>477132</v>
+        <v>664285</v>
       </c>
       <c r="C141" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2752,10 +2758,10 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>656302</v>
+        <v>686799</v>
       </c>
       <c r="C142" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2763,10 +2769,10 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>680694</v>
+        <v>666214</v>
       </c>
       <c r="C143" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2774,10 +2780,10 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>622491</v>
+        <v>608331</v>
       </c>
       <c r="C144" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2785,10 +2791,10 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>669022</v>
+        <v>666157</v>
       </c>
       <c r="C145" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2796,10 +2802,10 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>547179</v>
+        <v>672710</v>
       </c>
       <c r="C146" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2807,10 +2813,10 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>607259</v>
+        <v>660271</v>
       </c>
       <c r="C147" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2818,10 +2824,10 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>674370</v>
+        <v>680573</v>
       </c>
       <c r="C148" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2829,10 +2835,10 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>571578</v>
+        <v>677944</v>
       </c>
       <c r="C149" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2840,10 +2846,10 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>640455</v>
+        <v>506433</v>
       </c>
       <c r="C150" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2851,10 +2857,10 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>669358</v>
+        <v>687473</v>
       </c>
       <c r="C151" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2862,10 +2868,10 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>579328</v>
+        <v>686701</v>
       </c>
       <c r="C152" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2873,10 +2879,10 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>694819</v>
+        <v>656641</v>
       </c>
       <c r="C153" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2884,10 +2890,10 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>800048</v>
+        <v>690997</v>
       </c>
       <c r="C154" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2895,10 +2901,10 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>686218</v>
+        <v>696149</v>
       </c>
       <c r="C155" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2906,10 +2912,10 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>668881</v>
+        <v>477132</v>
       </c>
       <c r="C156" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2917,10 +2923,10 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>676664</v>
+        <v>669022</v>
       </c>
       <c r="C157" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2928,10 +2934,10 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>690916</v>
+        <v>547179</v>
       </c>
       <c r="C158" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2939,10 +2945,10 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>675911</v>
+        <v>607259</v>
       </c>
       <c r="C159" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2950,10 +2956,10 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>702070</v>
+        <v>674370</v>
       </c>
       <c r="C160" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2961,10 +2967,10 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>592791</v>
+        <v>686218</v>
       </c>
       <c r="C161" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2972,10 +2978,10 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>688107</v>
+        <v>676664</v>
       </c>
       <c r="C162" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2983,10 +2989,10 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>682052</v>
+        <v>690916</v>
       </c>
       <c r="C163" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2994,10 +3000,10 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>676083</v>
+        <v>702070</v>
       </c>
       <c r="C164" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3005,10 +3011,10 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>621244</v>
+        <v>592791</v>
       </c>
       <c r="C165" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3016,10 +3022,10 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>690953</v>
+        <v>688107</v>
       </c>
       <c r="C166" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3027,10 +3033,10 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>681347</v>
+        <v>682052</v>
       </c>
       <c r="C167" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3038,10 +3044,10 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>682929</v>
+        <v>676083</v>
       </c>
       <c r="C168" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3049,10 +3055,10 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>671212</v>
+        <v>621244</v>
       </c>
       <c r="C169" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3060,10 +3066,10 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>570632</v>
+        <v>690953</v>
       </c>
       <c r="C170" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3071,10 +3077,10 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>687064</v>
+        <v>681347</v>
       </c>
       <c r="C171" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3082,10 +3088,10 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>678022</v>
+        <v>682929</v>
       </c>
       <c r="C172" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3093,10 +3099,10 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>689017</v>
+        <v>671212</v>
       </c>
       <c r="C173" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3104,62 +3110,62 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>596295</v>
+        <v>570632</v>
       </c>
       <c r="C174" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>155</v>
+        <v>175</v>
+      </c>
+      <c r="B175">
+        <v>687064</v>
       </c>
       <c r="C175" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B176">
-        <v>621111</v>
+        <v>678022</v>
       </c>
       <c r="C176" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B177">
-        <v>694477</v>
+        <v>689017</v>
       </c>
       <c r="C177" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B178">
-        <v>678906</v>
+        <v>596295</v>
       </c>
       <c r="C178" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>178</v>
-      </c>
-      <c r="B179">
-        <v>571760</v>
+        <v>161</v>
       </c>
       <c r="C179" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3167,10 +3173,10 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <v>607200</v>
+        <v>621111</v>
       </c>
       <c r="C180" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3178,10 +3184,10 @@
         <v>180</v>
       </c>
       <c r="B181">
-        <v>543135</v>
+        <v>694477</v>
       </c>
       <c r="C181" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3189,10 +3195,10 @@
         <v>181</v>
       </c>
       <c r="B182">
-        <v>471911</v>
+        <v>571760</v>
       </c>
       <c r="C182" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3200,10 +3206,10 @@
         <v>182</v>
       </c>
       <c r="B183">
-        <v>663559</v>
+        <v>607200</v>
       </c>
       <c r="C183" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3211,10 +3217,10 @@
         <v>183</v>
       </c>
       <c r="B184">
-        <v>647336</v>
+        <v>543135</v>
       </c>
       <c r="C184" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3222,10 +3228,10 @@
         <v>184</v>
       </c>
       <c r="B185">
-        <v>701519</v>
+        <v>471911</v>
       </c>
       <c r="C185" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3233,10 +3239,10 @@
         <v>185</v>
       </c>
       <c r="B186">
-        <v>677958</v>
+        <v>663559</v>
       </c>
       <c r="C186" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3244,10 +3250,10 @@
         <v>186</v>
       </c>
       <c r="B187">
-        <v>573186</v>
+        <v>647336</v>
       </c>
       <c r="C187" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3255,10 +3261,10 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>686563</v>
+        <v>701519</v>
       </c>
       <c r="C188" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3266,10 +3272,10 @@
         <v>188</v>
       </c>
       <c r="B189">
-        <v>622663</v>
+        <v>677958</v>
       </c>
       <c r="C189" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3277,10 +3283,10 @@
         <v>189</v>
       </c>
       <c r="B190">
-        <v>687922</v>
+        <v>573186</v>
       </c>
       <c r="C190" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3288,10 +3294,10 @@
         <v>190</v>
       </c>
       <c r="B191">
-        <v>688138</v>
+        <v>686563</v>
       </c>
       <c r="C191" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3299,10 +3305,10 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>701487</v>
+        <v>622663</v>
       </c>
       <c r="C192" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3310,10 +3316,10 @@
         <v>192</v>
       </c>
       <c r="B193">
-        <v>687134</v>
+        <v>687922</v>
       </c>
       <c r="C193" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3321,10 +3327,10 @@
         <v>193</v>
       </c>
       <c r="B194">
-        <v>593423</v>
+        <v>688138</v>
       </c>
       <c r="C194" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3332,10 +3338,10 @@
         <v>194</v>
       </c>
       <c r="B195">
-        <v>448179</v>
+        <v>701487</v>
       </c>
       <c r="C195" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3343,10 +3349,10 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>621107</v>
+        <v>687134</v>
       </c>
       <c r="C196" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3354,10 +3360,10 @@
         <v>196</v>
       </c>
       <c r="B197">
-        <v>695505</v>
+        <v>593423</v>
       </c>
       <c r="C197" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3365,10 +3371,10 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>675512</v>
+        <v>448179</v>
       </c>
       <c r="C198" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3376,10 +3382,10 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>676962</v>
+        <v>621107</v>
       </c>
       <c r="C199" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3387,10 +3393,10 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>676282</v>
+        <v>695505</v>
       </c>
       <c r="C200" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3398,10 +3404,10 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>680732</v>
+        <v>675512</v>
       </c>
       <c r="C201" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3409,10 +3415,10 @@
         <v>201</v>
       </c>
       <c r="B202">
-        <v>554430</v>
+        <v>676962</v>
       </c>
       <c r="C202" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3420,10 +3426,10 @@
         <v>202</v>
       </c>
       <c r="B203">
-        <v>676467</v>
+        <v>676282</v>
       </c>
       <c r="C203" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3431,10 +3437,10 @@
         <v>203</v>
       </c>
       <c r="B204">
-        <v>656550</v>
+        <v>680732</v>
       </c>
       <c r="C204" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3442,10 +3448,10 @@
         <v>204</v>
       </c>
       <c r="B205">
-        <v>663460</v>
+        <v>554430</v>
       </c>
       <c r="C205" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3453,10 +3459,10 @@
         <v>205</v>
       </c>
       <c r="B206">
-        <v>681190</v>
+        <v>676467</v>
       </c>
       <c r="C206" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3464,10 +3470,10 @@
         <v>206</v>
       </c>
       <c r="B207">
-        <v>669721</v>
+        <v>656550</v>
       </c>
       <c r="C207" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3475,10 +3481,10 @@
         <v>207</v>
       </c>
       <c r="B208">
-        <v>701581</v>
+        <v>663460</v>
       </c>
       <c r="C208" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3486,10 +3492,10 @@
         <v>208</v>
       </c>
       <c r="B209">
-        <v>806185</v>
+        <v>681190</v>
       </c>
       <c r="C209" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3497,10 +3503,10 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>672456</v>
+        <v>669721</v>
       </c>
       <c r="C210" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -3508,10 +3514,10 @@
         <v>210</v>
       </c>
       <c r="B211">
-        <v>687888</v>
+        <v>701581</v>
       </c>
       <c r="C211" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3519,10 +3525,10 @@
         <v>211</v>
       </c>
       <c r="B212">
-        <v>681857</v>
+        <v>806185</v>
       </c>
       <c r="C212" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3530,10 +3536,10 @@
         <v>212</v>
       </c>
       <c r="B213">
-        <v>666171</v>
+        <v>672456</v>
       </c>
       <c r="C213" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3541,10 +3547,10 @@
         <v>213</v>
       </c>
       <c r="B214">
-        <v>663795</v>
+        <v>687888</v>
       </c>
       <c r="C214" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3552,10 +3558,10 @@
         <v>214</v>
       </c>
       <c r="B215">
-        <v>696136</v>
+        <v>681857</v>
       </c>
       <c r="C215" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3563,10 +3569,10 @@
         <v>215</v>
       </c>
       <c r="B216">
-        <v>680736</v>
+        <v>666171</v>
       </c>
       <c r="C216" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3574,10 +3580,10 @@
         <v>216</v>
       </c>
       <c r="B217">
-        <v>642216</v>
+        <v>663795</v>
       </c>
       <c r="C217" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3585,10 +3591,10 @@
         <v>217</v>
       </c>
       <c r="B218">
-        <v>621112</v>
+        <v>696136</v>
       </c>
       <c r="C218" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3596,10 +3602,10 @@
         <v>218</v>
       </c>
       <c r="B219">
-        <v>680885</v>
+        <v>680736</v>
       </c>
       <c r="C219" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3607,10 +3613,10 @@
         <v>219</v>
       </c>
       <c r="B220">
-        <v>605513</v>
+        <v>642216</v>
       </c>
       <c r="C220" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -3618,10 +3624,10 @@
         <v>220</v>
       </c>
       <c r="B221">
-        <v>641302</v>
+        <v>621112</v>
       </c>
       <c r="C221" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3629,10 +3635,10 @@
         <v>221</v>
       </c>
       <c r="B222">
-        <v>690928</v>
+        <v>680885</v>
       </c>
       <c r="C222" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3640,10 +3646,10 @@
         <v>222</v>
       </c>
       <c r="B223">
-        <v>694918</v>
+        <v>605513</v>
       </c>
       <c r="C223" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3651,10 +3657,10 @@
         <v>223</v>
       </c>
       <c r="B224">
-        <v>800311</v>
+        <v>641302</v>
       </c>
       <c r="C224" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3662,10 +3668,10 @@
         <v>224</v>
       </c>
       <c r="B225">
-        <v>592866</v>
+        <v>690928</v>
       </c>
       <c r="C225" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3673,10 +3679,10 @@
         <v>225</v>
       </c>
       <c r="B226">
-        <v>678024</v>
+        <v>694918</v>
       </c>
       <c r="C226" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3684,10 +3690,10 @@
         <v>226</v>
       </c>
       <c r="B227">
-        <v>642232</v>
+        <v>800311</v>
       </c>
       <c r="C227" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3695,10 +3701,10 @@
         <v>227</v>
       </c>
       <c r="B228">
-        <v>669422</v>
+        <v>592866</v>
       </c>
       <c r="C228" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3706,10 +3712,10 @@
         <v>228</v>
       </c>
       <c r="B229">
-        <v>657376</v>
+        <v>678024</v>
       </c>
       <c r="C229" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3717,10 +3723,10 @@
         <v>229</v>
       </c>
       <c r="B230">
-        <v>676508</v>
+        <v>642232</v>
       </c>
       <c r="C230" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3728,10 +3734,10 @@
         <v>230</v>
       </c>
       <c r="B231">
-        <v>687223</v>
+        <v>669422</v>
       </c>
       <c r="C231" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3739,10 +3745,10 @@
         <v>231</v>
       </c>
       <c r="B232">
-        <v>656288</v>
+        <v>657376</v>
       </c>
       <c r="C232" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3750,10 +3756,10 @@
         <v>232</v>
       </c>
       <c r="B233">
-        <v>690986</v>
+        <v>676508</v>
       </c>
       <c r="C233" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3761,10 +3767,10 @@
         <v>233</v>
       </c>
       <c r="B234">
-        <v>687765</v>
+        <v>687223</v>
       </c>
       <c r="C234" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3772,10 +3778,10 @@
         <v>234</v>
       </c>
       <c r="B235">
-        <v>641816</v>
+        <v>656288</v>
       </c>
       <c r="C235" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3783,10 +3789,10 @@
         <v>235</v>
       </c>
       <c r="B236">
-        <v>687830</v>
+        <v>690986</v>
       </c>
       <c r="C236" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3794,18 +3800,21 @@
         <v>236</v>
       </c>
       <c r="B237">
-        <v>676106</v>
+        <v>687765</v>
       </c>
       <c r="C237" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
         <v>237</v>
       </c>
+      <c r="B238">
+        <v>641816</v>
+      </c>
       <c r="C238" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3813,10 +3822,10 @@
         <v>238</v>
       </c>
       <c r="B239">
-        <v>489119</v>
+        <v>687830</v>
       </c>
       <c r="C239" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3824,10 +3833,10 @@
         <v>239</v>
       </c>
       <c r="B240">
-        <v>670102</v>
+        <v>676106</v>
       </c>
       <c r="C240" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3835,7 +3844,7 @@
         <v>240</v>
       </c>
       <c r="C241" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3843,10 +3852,10 @@
         <v>241</v>
       </c>
       <c r="B242">
-        <v>656731</v>
+        <v>489119</v>
       </c>
       <c r="C242" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3854,21 +3863,18 @@
         <v>242</v>
       </c>
       <c r="B243">
-        <v>676961</v>
+        <v>670102</v>
       </c>
       <c r="C243" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
         <v>243</v>
       </c>
-      <c r="B244">
-        <v>677960</v>
-      </c>
       <c r="C244" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3876,10 +3882,10 @@
         <v>244</v>
       </c>
       <c r="B245">
-        <v>605452</v>
+        <v>656731</v>
       </c>
       <c r="C245" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3887,10 +3893,10 @@
         <v>245</v>
       </c>
       <c r="B246">
-        <v>666142</v>
+        <v>676961</v>
       </c>
       <c r="C246" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3898,10 +3904,10 @@
         <v>246</v>
       </c>
       <c r="B247">
-        <v>689017</v>
+        <v>677960</v>
       </c>
       <c r="C247" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3909,10 +3915,10 @@
         <v>247</v>
       </c>
       <c r="B248">
-        <v>664062</v>
+        <v>605452</v>
       </c>
       <c r="C248" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3920,10 +3926,10 @@
         <v>248</v>
       </c>
       <c r="B249">
-        <v>676428</v>
+        <v>666142</v>
       </c>
       <c r="C249" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3931,10 +3937,10 @@
         <v>249</v>
       </c>
       <c r="B250">
-        <v>641154</v>
+        <v>689017</v>
       </c>
       <c r="C250" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3942,10 +3948,10 @@
         <v>250</v>
       </c>
       <c r="B251">
-        <v>676974</v>
+        <v>664062</v>
       </c>
       <c r="C251" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3953,10 +3959,10 @@
         <v>251</v>
       </c>
       <c r="B252">
-        <v>669203</v>
+        <v>676428</v>
       </c>
       <c r="C252" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3964,10 +3970,10 @@
         <v>252</v>
       </c>
       <c r="B253">
-        <v>680684</v>
+        <v>641154</v>
       </c>
       <c r="C253" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -3975,10 +3981,10 @@
         <v>253</v>
       </c>
       <c r="B254">
-        <v>700363</v>
+        <v>676974</v>
       </c>
       <c r="C254" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -3986,10 +3992,10 @@
         <v>254</v>
       </c>
       <c r="B255">
-        <v>663465</v>
+        <v>669203</v>
       </c>
       <c r="C255" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -3997,10 +4003,10 @@
         <v>255</v>
       </c>
       <c r="B256">
-        <v>695549</v>
+        <v>680684</v>
       </c>
       <c r="C256" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -4008,10 +4014,10 @@
         <v>256</v>
       </c>
       <c r="B257">
-        <v>663738</v>
+        <v>700363</v>
       </c>
       <c r="C257" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -4019,10 +4025,10 @@
         <v>257</v>
       </c>
       <c r="B258">
-        <v>701656</v>
+        <v>663465</v>
       </c>
       <c r="C258" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -4030,10 +4036,10 @@
         <v>258</v>
       </c>
       <c r="B259">
-        <v>650633</v>
+        <v>695549</v>
       </c>
       <c r="C259" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -4041,10 +4047,10 @@
         <v>259</v>
       </c>
       <c r="B260">
-        <v>694646</v>
+        <v>663738</v>
       </c>
       <c r="C260" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -4052,10 +4058,10 @@
         <v>260</v>
       </c>
       <c r="B261">
-        <v>669060</v>
+        <v>701656</v>
       </c>
       <c r="C261" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -4063,10 +4069,10 @@
         <v>261</v>
       </c>
       <c r="B262">
-        <v>669387</v>
+        <v>650633</v>
       </c>
       <c r="C262" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -4074,10 +4080,10 @@
         <v>262</v>
       </c>
       <c r="B263">
-        <v>502043</v>
+        <v>694646</v>
       </c>
       <c r="C263" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -4085,10 +4091,10 @@
         <v>263</v>
       </c>
       <c r="B264">
-        <v>669854</v>
+        <v>669387</v>
       </c>
       <c r="C264" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -4096,10 +4102,10 @@
         <v>264</v>
       </c>
       <c r="B265">
-        <v>668964</v>
+        <v>502043</v>
       </c>
       <c r="C265" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -4107,10 +4113,10 @@
         <v>265</v>
       </c>
       <c r="B266">
-        <v>695534</v>
+        <v>669854</v>
       </c>
       <c r="C266" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -4118,10 +4124,10 @@
         <v>266</v>
       </c>
       <c r="B267">
-        <v>663855</v>
+        <v>668964</v>
       </c>
       <c r="C267" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -4129,10 +4135,10 @@
         <v>267</v>
       </c>
       <c r="B268">
-        <v>678368</v>
+        <v>695534</v>
       </c>
       <c r="C268" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -4140,10 +4146,10 @@
         <v>268</v>
       </c>
       <c r="B269">
-        <v>594902</v>
+        <v>663855</v>
       </c>
       <c r="C269" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -4151,10 +4157,10 @@
         <v>269</v>
       </c>
       <c r="B270">
-        <v>656557</v>
+        <v>678368</v>
       </c>
       <c r="C270" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -4162,10 +4168,10 @@
         <v>270</v>
       </c>
       <c r="B271">
-        <v>669713</v>
+        <v>594902</v>
       </c>
       <c r="C271" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="272" spans="1:3">
@@ -4173,10 +4179,10 @@
         <v>271</v>
       </c>
       <c r="B272">
-        <v>663372</v>
+        <v>656557</v>
       </c>
       <c r="C272" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -4184,10 +4190,32 @@
         <v>272</v>
       </c>
       <c r="B273">
+        <v>669713</v>
+      </c>
+      <c r="C273" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" t="s">
+        <v>273</v>
+      </c>
+      <c r="B274">
+        <v>663372</v>
+      </c>
+      <c r="C274" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" t="s">
+        <v>274</v>
+      </c>
+      <c r="B275">
         <v>686249</v>
       </c>
-      <c r="C273" t="s">
-        <v>273</v>
+      <c r="C275" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>